<commit_message>
Atualização Gráfico de Gantt
</commit_message>
<xml_diff>
--- a/Gerência/Rogercard Gantt.xlsx
+++ b/Gerência/Rogercard Gantt.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>ATIVIDADE METODOLÓGICA</t>
   </si>
@@ -88,7 +88,16 @@
     <t>Revisão do diagrama de classe.</t>
   </si>
   <si>
+    <t>Revisão das classes e interface.</t>
+  </si>
+  <si>
     <t>ATIVIDADE CODIFICAÇÃO</t>
+  </si>
+  <si>
+    <t>Codificação das classes e interface.</t>
+  </si>
+  <si>
+    <t>Correção das classes e interface.</t>
   </si>
 </sst>
 </file>
@@ -117,7 +126,7 @@
     </font>
     <font>
       <sz val="10.0"/>
-      <color theme="0"/>
+      <color rgb="FF000000"/>
       <name val="Times New Roman"/>
     </font>
     <font>
@@ -149,7 +158,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <color rgb="FFF1C232"/>
+      <color rgb="FF000000"/>
       <name val="Times New Roman"/>
     </font>
   </fonts>
@@ -233,7 +242,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="30">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -246,7 +255,7 @@
     <xf borderId="0" fillId="2" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="3" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="3" fontId="3" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
@@ -284,11 +293,17 @@
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="10" fontId="7" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="10" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
     <xf borderId="0" fillId="11" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="12" fontId="10" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="12" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="12" fontId="9" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="12" fontId="7" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
@@ -301,6 +316,7 @@
     <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -665,10 +681,78 @@
       <c r="AU1" s="3">
         <v>45600.0</v>
       </c>
-      <c r="AV1" s="4"/>
-      <c r="AW1" s="4"/>
-      <c r="AX1" s="4"/>
-      <c r="AY1" s="4"/>
+      <c r="AV1" s="3">
+        <v>45601.0</v>
+      </c>
+      <c r="AW1" s="3">
+        <v>45602.0</v>
+      </c>
+      <c r="AX1" s="3">
+        <v>45603.0</v>
+      </c>
+      <c r="AY1" s="3">
+        <v>45604.0</v>
+      </c>
+      <c r="AZ1" s="4">
+        <v>45607.0</v>
+      </c>
+      <c r="BA1" s="4">
+        <v>45608.0</v>
+      </c>
+      <c r="BB1" s="4">
+        <v>45609.0</v>
+      </c>
+      <c r="BC1" s="4">
+        <v>45610.0</v>
+      </c>
+      <c r="BD1" s="4">
+        <v>45611.0</v>
+      </c>
+      <c r="BE1" s="3">
+        <v>45614.0</v>
+      </c>
+      <c r="BF1" s="3">
+        <v>45615.0</v>
+      </c>
+      <c r="BG1" s="3">
+        <v>45616.0</v>
+      </c>
+      <c r="BH1" s="3">
+        <v>45617.0</v>
+      </c>
+      <c r="BI1" s="3">
+        <v>45618.0</v>
+      </c>
+      <c r="BJ1" s="4">
+        <v>45621.0</v>
+      </c>
+      <c r="BK1" s="4">
+        <v>45622.0</v>
+      </c>
+      <c r="BL1" s="4">
+        <v>45623.0</v>
+      </c>
+      <c r="BM1" s="4">
+        <v>45624.0</v>
+      </c>
+      <c r="BN1" s="4">
+        <v>45625.0</v>
+      </c>
+      <c r="BO1" s="3">
+        <v>45628.0</v>
+      </c>
+      <c r="BP1" s="3">
+        <v>45629.0</v>
+      </c>
+      <c r="BQ1" s="3">
+        <v>45630.0</v>
+      </c>
+      <c r="BR1" s="3">
+        <v>45631.0</v>
+      </c>
+      <c r="BS1" s="3">
+        <v>45632.0</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="5" t="s">
@@ -724,6 +808,26 @@
       <c r="AW2" s="6"/>
       <c r="AX2" s="6"/>
       <c r="AY2" s="6"/>
+      <c r="AZ2" s="6"/>
+      <c r="BA2" s="6"/>
+      <c r="BB2" s="6"/>
+      <c r="BC2" s="6"/>
+      <c r="BD2" s="6"/>
+      <c r="BE2" s="6"/>
+      <c r="BF2" s="6"/>
+      <c r="BG2" s="6"/>
+      <c r="BH2" s="6"/>
+      <c r="BI2" s="6"/>
+      <c r="BJ2" s="6"/>
+      <c r="BK2" s="6"/>
+      <c r="BL2" s="6"/>
+      <c r="BM2" s="6"/>
+      <c r="BN2" s="6"/>
+      <c r="BO2" s="6"/>
+      <c r="BP2" s="6"/>
+      <c r="BQ2" s="6"/>
+      <c r="BR2" s="6"/>
+      <c r="BS2" s="6"/>
     </row>
     <row r="3">
       <c r="A3" s="7" t="s">
@@ -900,2926 +1004,2955 @@
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="21"/>
+      <c r="A27" s="21" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="28">
-      <c r="A28" s="22"/>
+      <c r="A28" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="AU28" s="23"/>
+      <c r="AV28" s="23"/>
+      <c r="AW28" s="23"/>
+      <c r="AX28" s="23"/>
+      <c r="AY28" s="23"/>
+      <c r="AZ28" s="23"/>
+      <c r="BA28" s="23"/>
+      <c r="BB28" s="23"/>
+      <c r="BC28" s="23"/>
+      <c r="BD28" s="23"/>
+      <c r="BE28" s="23"/>
+      <c r="BF28" s="23"/>
+      <c r="BG28" s="23"/>
+      <c r="BH28" s="23"/>
+      <c r="BI28" s="23"/>
+      <c r="BJ28" s="23"/>
+      <c r="BK28" s="23"/>
+      <c r="BL28" s="23"/>
+      <c r="BM28" s="23"/>
+      <c r="BN28" s="23"/>
+      <c r="BO28" s="23"/>
+      <c r="BP28" s="23"/>
+      <c r="BQ28" s="24"/>
     </row>
     <row r="29">
-      <c r="A29" s="22"/>
+      <c r="A29" s="22" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="30">
-      <c r="A30" s="23"/>
+      <c r="A30" s="25"/>
     </row>
     <row r="31">
-      <c r="A31" s="24"/>
+      <c r="A31" s="26"/>
     </row>
     <row r="32">
-      <c r="A32" s="24"/>
+      <c r="A32" s="26"/>
     </row>
     <row r="33">
-      <c r="A33" s="23"/>
+      <c r="A33" s="25"/>
     </row>
     <row r="34">
-      <c r="A34" s="23"/>
+      <c r="A34" s="25"/>
     </row>
     <row r="35">
-      <c r="A35" s="24"/>
+      <c r="A35" s="26"/>
     </row>
     <row r="36">
-      <c r="A36" s="24"/>
+      <c r="A36" s="26"/>
     </row>
     <row r="37">
-      <c r="A37" s="24"/>
+      <c r="A37" s="26"/>
     </row>
     <row r="38">
-      <c r="A38" s="24"/>
+      <c r="A38" s="26"/>
     </row>
     <row r="39">
-      <c r="A39" s="24"/>
+      <c r="A39" s="26"/>
     </row>
     <row r="40">
-      <c r="A40" s="24"/>
+      <c r="A40" s="26"/>
     </row>
     <row r="41">
-      <c r="A41" s="24"/>
+      <c r="A41" s="26"/>
     </row>
     <row r="42">
-      <c r="A42" s="24"/>
+      <c r="A42" s="26"/>
     </row>
     <row r="43">
-      <c r="A43" s="25"/>
+      <c r="A43" s="27"/>
     </row>
     <row r="44">
-      <c r="A44" s="26"/>
+      <c r="A44" s="28"/>
     </row>
     <row r="45">
-      <c r="A45" s="25"/>
+      <c r="A45" s="27"/>
     </row>
     <row r="46">
-      <c r="A46" s="25"/>
+      <c r="A46" s="27"/>
     </row>
     <row r="47">
-      <c r="A47" s="25"/>
+      <c r="A47" s="27"/>
     </row>
     <row r="48">
-      <c r="A48" s="25"/>
+      <c r="A48" s="27"/>
     </row>
     <row r="49">
-      <c r="A49" s="25"/>
+      <c r="A49" s="27"/>
     </row>
     <row r="50">
-      <c r="A50" s="25"/>
+      <c r="A50" s="27"/>
     </row>
     <row r="51">
-      <c r="A51" s="25"/>
+      <c r="A51" s="27"/>
     </row>
     <row r="52">
-      <c r="A52" s="24"/>
+      <c r="A52" s="26"/>
     </row>
     <row r="53">
-      <c r="A53" s="22"/>
+      <c r="A53" s="29"/>
     </row>
     <row r="54">
-      <c r="A54" s="22"/>
+      <c r="A54" s="29"/>
     </row>
     <row r="55">
-      <c r="A55" s="22"/>
+      <c r="A55" s="29"/>
     </row>
     <row r="56">
-      <c r="A56" s="22"/>
+      <c r="A56" s="29"/>
     </row>
     <row r="57">
-      <c r="A57" s="22"/>
+      <c r="A57" s="29"/>
     </row>
     <row r="58">
-      <c r="A58" s="22"/>
+      <c r="A58" s="29"/>
     </row>
     <row r="59">
-      <c r="A59" s="22"/>
+      <c r="A59" s="29"/>
     </row>
     <row r="60">
-      <c r="A60" s="22"/>
+      <c r="A60" s="29"/>
     </row>
     <row r="61">
-      <c r="A61" s="22"/>
+      <c r="A61" s="29"/>
     </row>
     <row r="62">
-      <c r="A62" s="22"/>
+      <c r="A62" s="29"/>
     </row>
     <row r="63">
-      <c r="A63" s="22"/>
+      <c r="A63" s="29"/>
     </row>
     <row r="64">
-      <c r="A64" s="22"/>
+      <c r="A64" s="29"/>
     </row>
     <row r="65">
-      <c r="A65" s="22"/>
+      <c r="A65" s="29"/>
     </row>
     <row r="66">
-      <c r="A66" s="22"/>
+      <c r="A66" s="29"/>
     </row>
     <row r="67">
-      <c r="A67" s="22"/>
+      <c r="A67" s="29"/>
     </row>
     <row r="68">
-      <c r="A68" s="22"/>
+      <c r="A68" s="29"/>
     </row>
     <row r="69">
-      <c r="A69" s="22"/>
+      <c r="A69" s="29"/>
     </row>
     <row r="70">
-      <c r="A70" s="22"/>
+      <c r="A70" s="29"/>
     </row>
     <row r="71">
-      <c r="A71" s="22"/>
+      <c r="A71" s="29"/>
     </row>
     <row r="72">
-      <c r="A72" s="22"/>
+      <c r="A72" s="29"/>
     </row>
     <row r="73">
-      <c r="A73" s="22"/>
+      <c r="A73" s="29"/>
     </row>
     <row r="74">
-      <c r="A74" s="22"/>
+      <c r="A74" s="29"/>
     </row>
     <row r="75">
-      <c r="A75" s="22"/>
+      <c r="A75" s="29"/>
     </row>
     <row r="76">
-      <c r="A76" s="22"/>
+      <c r="A76" s="29"/>
     </row>
     <row r="77">
-      <c r="A77" s="22"/>
+      <c r="A77" s="29"/>
     </row>
     <row r="78">
-      <c r="A78" s="22"/>
+      <c r="A78" s="29"/>
     </row>
     <row r="79">
-      <c r="A79" s="22"/>
+      <c r="A79" s="29"/>
     </row>
     <row r="80">
-      <c r="A80" s="22"/>
+      <c r="A80" s="29"/>
     </row>
     <row r="81">
-      <c r="A81" s="22"/>
+      <c r="A81" s="29"/>
     </row>
     <row r="82">
-      <c r="A82" s="22"/>
+      <c r="A82" s="29"/>
     </row>
     <row r="83">
-      <c r="A83" s="22"/>
+      <c r="A83" s="29"/>
     </row>
     <row r="84">
-      <c r="A84" s="22"/>
+      <c r="A84" s="29"/>
     </row>
     <row r="85">
-      <c r="A85" s="22"/>
+      <c r="A85" s="29"/>
     </row>
     <row r="86">
-      <c r="A86" s="22"/>
+      <c r="A86" s="29"/>
     </row>
     <row r="87">
-      <c r="A87" s="22"/>
+      <c r="A87" s="29"/>
     </row>
     <row r="88">
-      <c r="A88" s="22"/>
+      <c r="A88" s="29"/>
     </row>
     <row r="89">
-      <c r="A89" s="22"/>
+      <c r="A89" s="29"/>
     </row>
     <row r="90">
-      <c r="A90" s="22"/>
+      <c r="A90" s="29"/>
     </row>
     <row r="91">
-      <c r="A91" s="22"/>
+      <c r="A91" s="29"/>
     </row>
     <row r="92">
-      <c r="A92" s="22"/>
+      <c r="A92" s="29"/>
     </row>
     <row r="93">
-      <c r="A93" s="22"/>
+      <c r="A93" s="29"/>
     </row>
     <row r="94">
-      <c r="A94" s="22"/>
+      <c r="A94" s="29"/>
     </row>
     <row r="95">
-      <c r="A95" s="22"/>
+      <c r="A95" s="29"/>
     </row>
     <row r="96">
-      <c r="A96" s="22"/>
+      <c r="A96" s="29"/>
     </row>
     <row r="97">
-      <c r="A97" s="22"/>
+      <c r="A97" s="29"/>
     </row>
     <row r="98">
-      <c r="A98" s="22"/>
+      <c r="A98" s="29"/>
     </row>
     <row r="99">
-      <c r="A99" s="22"/>
+      <c r="A99" s="29"/>
     </row>
     <row r="100">
-      <c r="A100" s="22"/>
+      <c r="A100" s="29"/>
     </row>
     <row r="101">
-      <c r="A101" s="22"/>
+      <c r="A101" s="29"/>
     </row>
     <row r="102">
-      <c r="A102" s="22"/>
+      <c r="A102" s="29"/>
     </row>
     <row r="103">
-      <c r="A103" s="22"/>
+      <c r="A103" s="29"/>
     </row>
     <row r="104">
-      <c r="A104" s="22"/>
+      <c r="A104" s="29"/>
     </row>
     <row r="105">
-      <c r="A105" s="22"/>
+      <c r="A105" s="29"/>
     </row>
     <row r="106">
-      <c r="A106" s="22"/>
+      <c r="A106" s="29"/>
     </row>
     <row r="107">
-      <c r="A107" s="22"/>
+      <c r="A107" s="29"/>
     </row>
     <row r="108">
-      <c r="A108" s="22"/>
+      <c r="A108" s="29"/>
     </row>
     <row r="109">
-      <c r="A109" s="22"/>
+      <c r="A109" s="29"/>
     </row>
     <row r="110">
-      <c r="A110" s="22"/>
+      <c r="A110" s="29"/>
     </row>
     <row r="111">
-      <c r="A111" s="22"/>
+      <c r="A111" s="29"/>
     </row>
     <row r="112">
-      <c r="A112" s="22"/>
+      <c r="A112" s="29"/>
     </row>
     <row r="113">
-      <c r="A113" s="22"/>
+      <c r="A113" s="29"/>
     </row>
     <row r="114">
-      <c r="A114" s="22"/>
+      <c r="A114" s="29"/>
     </row>
     <row r="115">
-      <c r="A115" s="22"/>
+      <c r="A115" s="29"/>
     </row>
     <row r="116">
-      <c r="A116" s="22"/>
+      <c r="A116" s="29"/>
     </row>
     <row r="117">
-      <c r="A117" s="22"/>
+      <c r="A117" s="29"/>
     </row>
     <row r="118">
-      <c r="A118" s="22"/>
+      <c r="A118" s="29"/>
     </row>
     <row r="119">
-      <c r="A119" s="22"/>
+      <c r="A119" s="29"/>
     </row>
     <row r="120">
-      <c r="A120" s="22"/>
+      <c r="A120" s="29"/>
     </row>
     <row r="121">
-      <c r="A121" s="22"/>
+      <c r="A121" s="29"/>
     </row>
     <row r="122">
-      <c r="A122" s="22"/>
+      <c r="A122" s="29"/>
     </row>
     <row r="123">
-      <c r="A123" s="22"/>
+      <c r="A123" s="29"/>
     </row>
     <row r="124">
-      <c r="A124" s="22"/>
+      <c r="A124" s="29"/>
     </row>
     <row r="125">
-      <c r="A125" s="22"/>
+      <c r="A125" s="29"/>
     </row>
     <row r="126">
-      <c r="A126" s="22"/>
+      <c r="A126" s="29"/>
     </row>
     <row r="127">
-      <c r="A127" s="22"/>
+      <c r="A127" s="29"/>
     </row>
     <row r="128">
-      <c r="A128" s="22"/>
+      <c r="A128" s="29"/>
     </row>
     <row r="129">
-      <c r="A129" s="22"/>
+      <c r="A129" s="29"/>
     </row>
     <row r="130">
-      <c r="A130" s="22"/>
+      <c r="A130" s="29"/>
     </row>
     <row r="131">
-      <c r="A131" s="22"/>
+      <c r="A131" s="29"/>
     </row>
     <row r="132">
-      <c r="A132" s="22"/>
+      <c r="A132" s="29"/>
     </row>
     <row r="133">
-      <c r="A133" s="22"/>
+      <c r="A133" s="29"/>
     </row>
     <row r="134">
-      <c r="A134" s="22"/>
+      <c r="A134" s="29"/>
     </row>
     <row r="135">
-      <c r="A135" s="22"/>
+      <c r="A135" s="29"/>
     </row>
     <row r="136">
-      <c r="A136" s="22"/>
+      <c r="A136" s="29"/>
     </row>
     <row r="137">
-      <c r="A137" s="22"/>
+      <c r="A137" s="29"/>
     </row>
     <row r="138">
-      <c r="A138" s="22"/>
+      <c r="A138" s="29"/>
     </row>
     <row r="139">
-      <c r="A139" s="22"/>
+      <c r="A139" s="29"/>
     </row>
     <row r="140">
-      <c r="A140" s="22"/>
+      <c r="A140" s="29"/>
     </row>
     <row r="141">
-      <c r="A141" s="22"/>
+      <c r="A141" s="29"/>
     </row>
     <row r="142">
-      <c r="A142" s="22"/>
+      <c r="A142" s="29"/>
     </row>
     <row r="143">
-      <c r="A143" s="22"/>
+      <c r="A143" s="29"/>
     </row>
     <row r="144">
-      <c r="A144" s="22"/>
+      <c r="A144" s="29"/>
     </row>
     <row r="145">
-      <c r="A145" s="22"/>
+      <c r="A145" s="29"/>
     </row>
     <row r="146">
-      <c r="A146" s="22"/>
+      <c r="A146" s="29"/>
     </row>
     <row r="147">
-      <c r="A147" s="22"/>
+      <c r="A147" s="29"/>
     </row>
     <row r="148">
-      <c r="A148" s="22"/>
+      <c r="A148" s="29"/>
     </row>
     <row r="149">
-      <c r="A149" s="22"/>
+      <c r="A149" s="29"/>
     </row>
     <row r="150">
-      <c r="A150" s="22"/>
+      <c r="A150" s="29"/>
     </row>
     <row r="151">
-      <c r="A151" s="22"/>
+      <c r="A151" s="29"/>
     </row>
     <row r="152">
-      <c r="A152" s="22"/>
+      <c r="A152" s="29"/>
     </row>
     <row r="153">
-      <c r="A153" s="22"/>
+      <c r="A153" s="29"/>
     </row>
     <row r="154">
-      <c r="A154" s="22"/>
+      <c r="A154" s="29"/>
     </row>
     <row r="155">
-      <c r="A155" s="22"/>
+      <c r="A155" s="29"/>
     </row>
     <row r="156">
-      <c r="A156" s="22"/>
+      <c r="A156" s="29"/>
     </row>
     <row r="157">
-      <c r="A157" s="22"/>
+      <c r="A157" s="29"/>
     </row>
     <row r="158">
-      <c r="A158" s="22"/>
+      <c r="A158" s="29"/>
     </row>
     <row r="159">
-      <c r="A159" s="22"/>
+      <c r="A159" s="29"/>
     </row>
     <row r="160">
-      <c r="A160" s="22"/>
+      <c r="A160" s="29"/>
     </row>
     <row r="161">
-      <c r="A161" s="22"/>
+      <c r="A161" s="29"/>
     </row>
     <row r="162">
-      <c r="A162" s="22"/>
+      <c r="A162" s="29"/>
     </row>
     <row r="163">
-      <c r="A163" s="22"/>
+      <c r="A163" s="29"/>
     </row>
     <row r="164">
-      <c r="A164" s="22"/>
+      <c r="A164" s="29"/>
     </row>
     <row r="165">
-      <c r="A165" s="22"/>
+      <c r="A165" s="29"/>
     </row>
     <row r="166">
-      <c r="A166" s="22"/>
+      <c r="A166" s="29"/>
     </row>
     <row r="167">
-      <c r="A167" s="22"/>
+      <c r="A167" s="29"/>
     </row>
     <row r="168">
-      <c r="A168" s="22"/>
+      <c r="A168" s="29"/>
     </row>
     <row r="169">
-      <c r="A169" s="22"/>
+      <c r="A169" s="29"/>
     </row>
     <row r="170">
-      <c r="A170" s="22"/>
+      <c r="A170" s="29"/>
     </row>
     <row r="171">
-      <c r="A171" s="22"/>
+      <c r="A171" s="29"/>
     </row>
     <row r="172">
-      <c r="A172" s="22"/>
+      <c r="A172" s="29"/>
     </row>
     <row r="173">
-      <c r="A173" s="22"/>
+      <c r="A173" s="29"/>
     </row>
     <row r="174">
-      <c r="A174" s="22"/>
+      <c r="A174" s="29"/>
     </row>
     <row r="175">
-      <c r="A175" s="22"/>
+      <c r="A175" s="29"/>
     </row>
     <row r="176">
-      <c r="A176" s="22"/>
+      <c r="A176" s="29"/>
     </row>
     <row r="177">
-      <c r="A177" s="22"/>
+      <c r="A177" s="29"/>
     </row>
     <row r="178">
-      <c r="A178" s="22"/>
+      <c r="A178" s="29"/>
     </row>
     <row r="179">
-      <c r="A179" s="22"/>
+      <c r="A179" s="29"/>
     </row>
     <row r="180">
-      <c r="A180" s="22"/>
+      <c r="A180" s="29"/>
     </row>
     <row r="181">
-      <c r="A181" s="22"/>
+      <c r="A181" s="29"/>
     </row>
     <row r="182">
-      <c r="A182" s="22"/>
+      <c r="A182" s="29"/>
     </row>
     <row r="183">
-      <c r="A183" s="22"/>
+      <c r="A183" s="29"/>
     </row>
     <row r="184">
-      <c r="A184" s="22"/>
+      <c r="A184" s="29"/>
     </row>
     <row r="185">
-      <c r="A185" s="22"/>
+      <c r="A185" s="29"/>
     </row>
     <row r="186">
-      <c r="A186" s="22"/>
+      <c r="A186" s="29"/>
     </row>
     <row r="187">
-      <c r="A187" s="22"/>
+      <c r="A187" s="29"/>
     </row>
     <row r="188">
-      <c r="A188" s="22"/>
+      <c r="A188" s="29"/>
     </row>
     <row r="189">
-      <c r="A189" s="22"/>
+      <c r="A189" s="29"/>
     </row>
     <row r="190">
-      <c r="A190" s="22"/>
+      <c r="A190" s="29"/>
     </row>
     <row r="191">
-      <c r="A191" s="22"/>
+      <c r="A191" s="29"/>
     </row>
     <row r="192">
-      <c r="A192" s="22"/>
+      <c r="A192" s="29"/>
     </row>
     <row r="193">
-      <c r="A193" s="22"/>
+      <c r="A193" s="29"/>
     </row>
     <row r="194">
-      <c r="A194" s="22"/>
+      <c r="A194" s="29"/>
     </row>
     <row r="195">
-      <c r="A195" s="22"/>
+      <c r="A195" s="29"/>
     </row>
     <row r="196">
-      <c r="A196" s="22"/>
+      <c r="A196" s="29"/>
     </row>
     <row r="197">
-      <c r="A197" s="22"/>
+      <c r="A197" s="29"/>
     </row>
     <row r="198">
-      <c r="A198" s="22"/>
+      <c r="A198" s="29"/>
     </row>
     <row r="199">
-      <c r="A199" s="22"/>
+      <c r="A199" s="29"/>
     </row>
     <row r="200">
-      <c r="A200" s="22"/>
+      <c r="A200" s="29"/>
     </row>
     <row r="201">
-      <c r="A201" s="22"/>
+      <c r="A201" s="29"/>
     </row>
     <row r="202">
-      <c r="A202" s="22"/>
+      <c r="A202" s="29"/>
     </row>
     <row r="203">
-      <c r="A203" s="22"/>
+      <c r="A203" s="29"/>
     </row>
     <row r="204">
-      <c r="A204" s="22"/>
+      <c r="A204" s="29"/>
     </row>
     <row r="205">
-      <c r="A205" s="22"/>
+      <c r="A205" s="29"/>
     </row>
     <row r="206">
-      <c r="A206" s="22"/>
+      <c r="A206" s="29"/>
     </row>
     <row r="207">
-      <c r="A207" s="22"/>
+      <c r="A207" s="29"/>
     </row>
     <row r="208">
-      <c r="A208" s="22"/>
+      <c r="A208" s="29"/>
     </row>
     <row r="209">
-      <c r="A209" s="22"/>
+      <c r="A209" s="29"/>
     </row>
     <row r="210">
-      <c r="A210" s="22"/>
+      <c r="A210" s="29"/>
     </row>
     <row r="211">
-      <c r="A211" s="22"/>
+      <c r="A211" s="29"/>
     </row>
     <row r="212">
-      <c r="A212" s="22"/>
+      <c r="A212" s="29"/>
     </row>
     <row r="213">
-      <c r="A213" s="22"/>
+      <c r="A213" s="29"/>
     </row>
     <row r="214">
-      <c r="A214" s="22"/>
+      <c r="A214" s="29"/>
     </row>
     <row r="215">
-      <c r="A215" s="22"/>
+      <c r="A215" s="29"/>
     </row>
     <row r="216">
-      <c r="A216" s="22"/>
+      <c r="A216" s="29"/>
     </row>
     <row r="217">
-      <c r="A217" s="22"/>
+      <c r="A217" s="29"/>
     </row>
     <row r="218">
-      <c r="A218" s="22"/>
+      <c r="A218" s="29"/>
     </row>
     <row r="219">
-      <c r="A219" s="22"/>
+      <c r="A219" s="29"/>
     </row>
     <row r="220">
-      <c r="A220" s="22"/>
+      <c r="A220" s="29"/>
     </row>
     <row r="221">
-      <c r="A221" s="22"/>
+      <c r="A221" s="29"/>
     </row>
     <row r="222">
-      <c r="A222" s="22"/>
+      <c r="A222" s="29"/>
     </row>
     <row r="223">
-      <c r="A223" s="22"/>
+      <c r="A223" s="29"/>
     </row>
     <row r="224">
-      <c r="A224" s="22"/>
+      <c r="A224" s="29"/>
     </row>
     <row r="225">
-      <c r="A225" s="22"/>
+      <c r="A225" s="29"/>
     </row>
     <row r="226">
-      <c r="A226" s="22"/>
+      <c r="A226" s="29"/>
     </row>
     <row r="227">
-      <c r="A227" s="22"/>
+      <c r="A227" s="29"/>
     </row>
     <row r="228">
-      <c r="A228" s="22"/>
+      <c r="A228" s="29"/>
     </row>
     <row r="229">
-      <c r="A229" s="22"/>
+      <c r="A229" s="29"/>
     </row>
     <row r="230">
-      <c r="A230" s="22"/>
+      <c r="A230" s="29"/>
     </row>
     <row r="231">
-      <c r="A231" s="22"/>
+      <c r="A231" s="29"/>
     </row>
     <row r="232">
-      <c r="A232" s="22"/>
+      <c r="A232" s="29"/>
     </row>
     <row r="233">
-      <c r="A233" s="22"/>
+      <c r="A233" s="29"/>
     </row>
     <row r="234">
-      <c r="A234" s="22"/>
+      <c r="A234" s="29"/>
     </row>
     <row r="235">
-      <c r="A235" s="22"/>
+      <c r="A235" s="29"/>
     </row>
     <row r="236">
-      <c r="A236" s="22"/>
+      <c r="A236" s="29"/>
     </row>
     <row r="237">
-      <c r="A237" s="22"/>
+      <c r="A237" s="29"/>
     </row>
     <row r="238">
-      <c r="A238" s="22"/>
+      <c r="A238" s="29"/>
     </row>
     <row r="239">
-      <c r="A239" s="22"/>
+      <c r="A239" s="29"/>
     </row>
     <row r="240">
-      <c r="A240" s="22"/>
+      <c r="A240" s="29"/>
     </row>
     <row r="241">
-      <c r="A241" s="22"/>
+      <c r="A241" s="29"/>
     </row>
     <row r="242">
-      <c r="A242" s="22"/>
+      <c r="A242" s="29"/>
     </row>
     <row r="243">
-      <c r="A243" s="22"/>
+      <c r="A243" s="29"/>
     </row>
     <row r="244">
-      <c r="A244" s="22"/>
+      <c r="A244" s="29"/>
     </row>
     <row r="245">
-      <c r="A245" s="22"/>
+      <c r="A245" s="29"/>
     </row>
     <row r="246">
-      <c r="A246" s="22"/>
+      <c r="A246" s="29"/>
     </row>
     <row r="247">
-      <c r="A247" s="22"/>
+      <c r="A247" s="29"/>
     </row>
     <row r="248">
-      <c r="A248" s="22"/>
+      <c r="A248" s="29"/>
     </row>
     <row r="249">
-      <c r="A249" s="22"/>
+      <c r="A249" s="29"/>
     </row>
     <row r="250">
-      <c r="A250" s="22"/>
+      <c r="A250" s="29"/>
     </row>
     <row r="251">
-      <c r="A251" s="22"/>
+      <c r="A251" s="29"/>
     </row>
     <row r="252">
-      <c r="A252" s="22"/>
+      <c r="A252" s="29"/>
     </row>
     <row r="253">
-      <c r="A253" s="22"/>
+      <c r="A253" s="29"/>
     </row>
     <row r="254">
-      <c r="A254" s="22"/>
+      <c r="A254" s="29"/>
     </row>
     <row r="255">
-      <c r="A255" s="22"/>
+      <c r="A255" s="29"/>
     </row>
     <row r="256">
-      <c r="A256" s="22"/>
+      <c r="A256" s="29"/>
     </row>
     <row r="257">
-      <c r="A257" s="22"/>
+      <c r="A257" s="29"/>
     </row>
     <row r="258">
-      <c r="A258" s="22"/>
+      <c r="A258" s="29"/>
     </row>
     <row r="259">
-      <c r="A259" s="22"/>
+      <c r="A259" s="29"/>
     </row>
     <row r="260">
-      <c r="A260" s="22"/>
+      <c r="A260" s="29"/>
     </row>
     <row r="261">
-      <c r="A261" s="22"/>
+      <c r="A261" s="29"/>
     </row>
     <row r="262">
-      <c r="A262" s="22"/>
+      <c r="A262" s="29"/>
     </row>
     <row r="263">
-      <c r="A263" s="22"/>
+      <c r="A263" s="29"/>
     </row>
     <row r="264">
-      <c r="A264" s="22"/>
+      <c r="A264" s="29"/>
     </row>
     <row r="265">
-      <c r="A265" s="22"/>
+      <c r="A265" s="29"/>
     </row>
     <row r="266">
-      <c r="A266" s="22"/>
+      <c r="A266" s="29"/>
     </row>
     <row r="267">
-      <c r="A267" s="22"/>
+      <c r="A267" s="29"/>
     </row>
     <row r="268">
-      <c r="A268" s="22"/>
+      <c r="A268" s="29"/>
     </row>
     <row r="269">
-      <c r="A269" s="22"/>
+      <c r="A269" s="29"/>
     </row>
     <row r="270">
-      <c r="A270" s="22"/>
+      <c r="A270" s="29"/>
     </row>
     <row r="271">
-      <c r="A271" s="22"/>
+      <c r="A271" s="29"/>
     </row>
     <row r="272">
-      <c r="A272" s="22"/>
+      <c r="A272" s="29"/>
     </row>
     <row r="273">
-      <c r="A273" s="22"/>
+      <c r="A273" s="29"/>
     </row>
     <row r="274">
-      <c r="A274" s="22"/>
+      <c r="A274" s="29"/>
     </row>
     <row r="275">
-      <c r="A275" s="22"/>
+      <c r="A275" s="29"/>
     </row>
     <row r="276">
-      <c r="A276" s="22"/>
+      <c r="A276" s="29"/>
     </row>
     <row r="277">
-      <c r="A277" s="22"/>
+      <c r="A277" s="29"/>
     </row>
     <row r="278">
-      <c r="A278" s="22"/>
+      <c r="A278" s="29"/>
     </row>
     <row r="279">
-      <c r="A279" s="22"/>
+      <c r="A279" s="29"/>
     </row>
     <row r="280">
-      <c r="A280" s="22"/>
+      <c r="A280" s="29"/>
     </row>
     <row r="281">
-      <c r="A281" s="22"/>
+      <c r="A281" s="29"/>
     </row>
     <row r="282">
-      <c r="A282" s="22"/>
+      <c r="A282" s="29"/>
     </row>
     <row r="283">
-      <c r="A283" s="22"/>
+      <c r="A283" s="29"/>
     </row>
     <row r="284">
-      <c r="A284" s="22"/>
+      <c r="A284" s="29"/>
     </row>
     <row r="285">
-      <c r="A285" s="22"/>
+      <c r="A285" s="29"/>
     </row>
     <row r="286">
-      <c r="A286" s="22"/>
+      <c r="A286" s="29"/>
     </row>
     <row r="287">
-      <c r="A287" s="22"/>
+      <c r="A287" s="29"/>
     </row>
     <row r="288">
-      <c r="A288" s="22"/>
+      <c r="A288" s="29"/>
     </row>
     <row r="289">
-      <c r="A289" s="22"/>
+      <c r="A289" s="29"/>
     </row>
     <row r="290">
-      <c r="A290" s="22"/>
+      <c r="A290" s="29"/>
     </row>
     <row r="291">
-      <c r="A291" s="22"/>
+      <c r="A291" s="29"/>
     </row>
     <row r="292">
-      <c r="A292" s="22"/>
+      <c r="A292" s="29"/>
     </row>
     <row r="293">
-      <c r="A293" s="22"/>
+      <c r="A293" s="29"/>
     </row>
     <row r="294">
-      <c r="A294" s="22"/>
+      <c r="A294" s="29"/>
     </row>
     <row r="295">
-      <c r="A295" s="22"/>
+      <c r="A295" s="29"/>
     </row>
     <row r="296">
-      <c r="A296" s="22"/>
+      <c r="A296" s="29"/>
     </row>
     <row r="297">
-      <c r="A297" s="22"/>
+      <c r="A297" s="29"/>
     </row>
     <row r="298">
-      <c r="A298" s="22"/>
+      <c r="A298" s="29"/>
     </row>
     <row r="299">
-      <c r="A299" s="22"/>
+      <c r="A299" s="29"/>
     </row>
     <row r="300">
-      <c r="A300" s="22"/>
+      <c r="A300" s="29"/>
     </row>
     <row r="301">
-      <c r="A301" s="22"/>
+      <c r="A301" s="29"/>
     </row>
     <row r="302">
-      <c r="A302" s="22"/>
+      <c r="A302" s="29"/>
     </row>
     <row r="303">
-      <c r="A303" s="22"/>
+      <c r="A303" s="29"/>
     </row>
     <row r="304">
-      <c r="A304" s="22"/>
+      <c r="A304" s="29"/>
     </row>
     <row r="305">
-      <c r="A305" s="22"/>
+      <c r="A305" s="29"/>
     </row>
     <row r="306">
-      <c r="A306" s="22"/>
+      <c r="A306" s="29"/>
     </row>
     <row r="307">
-      <c r="A307" s="22"/>
+      <c r="A307" s="29"/>
     </row>
     <row r="308">
-      <c r="A308" s="22"/>
+      <c r="A308" s="29"/>
     </row>
     <row r="309">
-      <c r="A309" s="22"/>
+      <c r="A309" s="29"/>
     </row>
     <row r="310">
-      <c r="A310" s="22"/>
+      <c r="A310" s="29"/>
     </row>
     <row r="311">
-      <c r="A311" s="22"/>
+      <c r="A311" s="29"/>
     </row>
     <row r="312">
-      <c r="A312" s="22"/>
+      <c r="A312" s="29"/>
     </row>
     <row r="313">
-      <c r="A313" s="22"/>
+      <c r="A313" s="29"/>
     </row>
     <row r="314">
-      <c r="A314" s="22"/>
+      <c r="A314" s="29"/>
     </row>
     <row r="315">
-      <c r="A315" s="22"/>
+      <c r="A315" s="29"/>
     </row>
     <row r="316">
-      <c r="A316" s="22"/>
+      <c r="A316" s="29"/>
     </row>
     <row r="317">
-      <c r="A317" s="22"/>
+      <c r="A317" s="29"/>
     </row>
     <row r="318">
-      <c r="A318" s="22"/>
+      <c r="A318" s="29"/>
     </row>
     <row r="319">
-      <c r="A319" s="22"/>
+      <c r="A319" s="29"/>
     </row>
     <row r="320">
-      <c r="A320" s="22"/>
+      <c r="A320" s="29"/>
     </row>
     <row r="321">
-      <c r="A321" s="22"/>
+      <c r="A321" s="29"/>
     </row>
     <row r="322">
-      <c r="A322" s="22"/>
+      <c r="A322" s="29"/>
     </row>
     <row r="323">
-      <c r="A323" s="22"/>
+      <c r="A323" s="29"/>
     </row>
     <row r="324">
-      <c r="A324" s="22"/>
+      <c r="A324" s="29"/>
     </row>
     <row r="325">
-      <c r="A325" s="22"/>
+      <c r="A325" s="29"/>
     </row>
     <row r="326">
-      <c r="A326" s="22"/>
+      <c r="A326" s="29"/>
     </row>
     <row r="327">
-      <c r="A327" s="22"/>
+      <c r="A327" s="29"/>
     </row>
     <row r="328">
-      <c r="A328" s="22"/>
+      <c r="A328" s="29"/>
     </row>
     <row r="329">
-      <c r="A329" s="22"/>
+      <c r="A329" s="29"/>
     </row>
     <row r="330">
-      <c r="A330" s="22"/>
+      <c r="A330" s="29"/>
     </row>
     <row r="331">
-      <c r="A331" s="22"/>
+      <c r="A331" s="29"/>
     </row>
     <row r="332">
-      <c r="A332" s="22"/>
+      <c r="A332" s="29"/>
     </row>
     <row r="333">
-      <c r="A333" s="22"/>
+      <c r="A333" s="29"/>
     </row>
     <row r="334">
-      <c r="A334" s="22"/>
+      <c r="A334" s="29"/>
     </row>
     <row r="335">
-      <c r="A335" s="22"/>
+      <c r="A335" s="29"/>
     </row>
     <row r="336">
-      <c r="A336" s="22"/>
+      <c r="A336" s="29"/>
     </row>
     <row r="337">
-      <c r="A337" s="22"/>
+      <c r="A337" s="29"/>
     </row>
     <row r="338">
-      <c r="A338" s="22"/>
+      <c r="A338" s="29"/>
     </row>
     <row r="339">
-      <c r="A339" s="22"/>
+      <c r="A339" s="29"/>
     </row>
     <row r="340">
-      <c r="A340" s="22"/>
+      <c r="A340" s="29"/>
     </row>
     <row r="341">
-      <c r="A341" s="22"/>
+      <c r="A341" s="29"/>
     </row>
     <row r="342">
-      <c r="A342" s="22"/>
+      <c r="A342" s="29"/>
     </row>
     <row r="343">
-      <c r="A343" s="22"/>
+      <c r="A343" s="29"/>
     </row>
     <row r="344">
-      <c r="A344" s="22"/>
+      <c r="A344" s="29"/>
     </row>
     <row r="345">
-      <c r="A345" s="22"/>
+      <c r="A345" s="29"/>
     </row>
     <row r="346">
-      <c r="A346" s="22"/>
+      <c r="A346" s="29"/>
     </row>
     <row r="347">
-      <c r="A347" s="22"/>
+      <c r="A347" s="29"/>
     </row>
     <row r="348">
-      <c r="A348" s="22"/>
+      <c r="A348" s="29"/>
     </row>
     <row r="349">
-      <c r="A349" s="22"/>
+      <c r="A349" s="29"/>
     </row>
     <row r="350">
-      <c r="A350" s="22"/>
+      <c r="A350" s="29"/>
     </row>
     <row r="351">
-      <c r="A351" s="22"/>
+      <c r="A351" s="29"/>
     </row>
     <row r="352">
-      <c r="A352" s="22"/>
+      <c r="A352" s="29"/>
     </row>
     <row r="353">
-      <c r="A353" s="22"/>
+      <c r="A353" s="29"/>
     </row>
     <row r="354">
-      <c r="A354" s="22"/>
+      <c r="A354" s="29"/>
     </row>
     <row r="355">
-      <c r="A355" s="22"/>
+      <c r="A355" s="29"/>
     </row>
     <row r="356">
-      <c r="A356" s="22"/>
+      <c r="A356" s="29"/>
     </row>
     <row r="357">
-      <c r="A357" s="22"/>
+      <c r="A357" s="29"/>
     </row>
     <row r="358">
-      <c r="A358" s="22"/>
+      <c r="A358" s="29"/>
     </row>
     <row r="359">
-      <c r="A359" s="22"/>
+      <c r="A359" s="29"/>
     </row>
     <row r="360">
-      <c r="A360" s="22"/>
+      <c r="A360" s="29"/>
     </row>
     <row r="361">
-      <c r="A361" s="22"/>
+      <c r="A361" s="29"/>
     </row>
     <row r="362">
-      <c r="A362" s="22"/>
+      <c r="A362" s="29"/>
     </row>
     <row r="363">
-      <c r="A363" s="22"/>
+      <c r="A363" s="29"/>
     </row>
     <row r="364">
-      <c r="A364" s="22"/>
+      <c r="A364" s="29"/>
     </row>
     <row r="365">
-      <c r="A365" s="22"/>
+      <c r="A365" s="29"/>
     </row>
     <row r="366">
-      <c r="A366" s="22"/>
+      <c r="A366" s="29"/>
     </row>
     <row r="367">
-      <c r="A367" s="22"/>
+      <c r="A367" s="29"/>
     </row>
     <row r="368">
-      <c r="A368" s="22"/>
+      <c r="A368" s="29"/>
     </row>
     <row r="369">
-      <c r="A369" s="22"/>
+      <c r="A369" s="29"/>
     </row>
     <row r="370">
-      <c r="A370" s="22"/>
+      <c r="A370" s="29"/>
     </row>
     <row r="371">
-      <c r="A371" s="22"/>
+      <c r="A371" s="29"/>
     </row>
     <row r="372">
-      <c r="A372" s="22"/>
+      <c r="A372" s="29"/>
     </row>
     <row r="373">
-      <c r="A373" s="22"/>
+      <c r="A373" s="29"/>
     </row>
     <row r="374">
-      <c r="A374" s="22"/>
+      <c r="A374" s="29"/>
     </row>
     <row r="375">
-      <c r="A375" s="22"/>
+      <c r="A375" s="29"/>
     </row>
     <row r="376">
-      <c r="A376" s="22"/>
+      <c r="A376" s="29"/>
     </row>
     <row r="377">
-      <c r="A377" s="22"/>
+      <c r="A377" s="29"/>
     </row>
     <row r="378">
-      <c r="A378" s="22"/>
+      <c r="A378" s="29"/>
     </row>
     <row r="379">
-      <c r="A379" s="22"/>
+      <c r="A379" s="29"/>
     </row>
     <row r="380">
-      <c r="A380" s="22"/>
+      <c r="A380" s="29"/>
     </row>
     <row r="381">
-      <c r="A381" s="22"/>
+      <c r="A381" s="29"/>
     </row>
     <row r="382">
-      <c r="A382" s="22"/>
+      <c r="A382" s="29"/>
     </row>
     <row r="383">
-      <c r="A383" s="22"/>
+      <c r="A383" s="29"/>
     </row>
     <row r="384">
-      <c r="A384" s="22"/>
+      <c r="A384" s="29"/>
     </row>
     <row r="385">
-      <c r="A385" s="22"/>
+      <c r="A385" s="29"/>
     </row>
     <row r="386">
-      <c r="A386" s="22"/>
+      <c r="A386" s="29"/>
     </row>
     <row r="387">
-      <c r="A387" s="22"/>
+      <c r="A387" s="29"/>
     </row>
     <row r="388">
-      <c r="A388" s="22"/>
+      <c r="A388" s="29"/>
     </row>
     <row r="389">
-      <c r="A389" s="22"/>
+      <c r="A389" s="29"/>
     </row>
     <row r="390">
-      <c r="A390" s="22"/>
+      <c r="A390" s="29"/>
     </row>
     <row r="391">
-      <c r="A391" s="22"/>
+      <c r="A391" s="29"/>
     </row>
     <row r="392">
-      <c r="A392" s="22"/>
+      <c r="A392" s="29"/>
     </row>
     <row r="393">
-      <c r="A393" s="22"/>
+      <c r="A393" s="29"/>
     </row>
     <row r="394">
-      <c r="A394" s="22"/>
+      <c r="A394" s="29"/>
     </row>
     <row r="395">
-      <c r="A395" s="22"/>
+      <c r="A395" s="29"/>
     </row>
     <row r="396">
-      <c r="A396" s="22"/>
+      <c r="A396" s="29"/>
     </row>
     <row r="397">
-      <c r="A397" s="22"/>
+      <c r="A397" s="29"/>
     </row>
     <row r="398">
-      <c r="A398" s="22"/>
+      <c r="A398" s="29"/>
     </row>
     <row r="399">
-      <c r="A399" s="22"/>
+      <c r="A399" s="29"/>
     </row>
     <row r="400">
-      <c r="A400" s="22"/>
+      <c r="A400" s="29"/>
     </row>
     <row r="401">
-      <c r="A401" s="22"/>
+      <c r="A401" s="29"/>
     </row>
     <row r="402">
-      <c r="A402" s="22"/>
+      <c r="A402" s="29"/>
     </row>
     <row r="403">
-      <c r="A403" s="22"/>
+      <c r="A403" s="29"/>
     </row>
     <row r="404">
-      <c r="A404" s="22"/>
+      <c r="A404" s="29"/>
     </row>
     <row r="405">
-      <c r="A405" s="22"/>
+      <c r="A405" s="29"/>
     </row>
     <row r="406">
-      <c r="A406" s="22"/>
+      <c r="A406" s="29"/>
     </row>
     <row r="407">
-      <c r="A407" s="22"/>
+      <c r="A407" s="29"/>
     </row>
     <row r="408">
-      <c r="A408" s="22"/>
+      <c r="A408" s="29"/>
     </row>
     <row r="409">
-      <c r="A409" s="22"/>
+      <c r="A409" s="29"/>
     </row>
     <row r="410">
-      <c r="A410" s="22"/>
+      <c r="A410" s="29"/>
     </row>
     <row r="411">
-      <c r="A411" s="22"/>
+      <c r="A411" s="29"/>
     </row>
     <row r="412">
-      <c r="A412" s="22"/>
+      <c r="A412" s="29"/>
     </row>
     <row r="413">
-      <c r="A413" s="22"/>
+      <c r="A413" s="29"/>
     </row>
     <row r="414">
-      <c r="A414" s="22"/>
+      <c r="A414" s="29"/>
     </row>
     <row r="415">
-      <c r="A415" s="22"/>
+      <c r="A415" s="29"/>
     </row>
     <row r="416">
-      <c r="A416" s="22"/>
+      <c r="A416" s="29"/>
     </row>
     <row r="417">
-      <c r="A417" s="22"/>
+      <c r="A417" s="29"/>
     </row>
     <row r="418">
-      <c r="A418" s="22"/>
+      <c r="A418" s="29"/>
     </row>
     <row r="419">
-      <c r="A419" s="22"/>
+      <c r="A419" s="29"/>
     </row>
     <row r="420">
-      <c r="A420" s="22"/>
+      <c r="A420" s="29"/>
     </row>
     <row r="421">
-      <c r="A421" s="22"/>
+      <c r="A421" s="29"/>
     </row>
     <row r="422">
-      <c r="A422" s="22"/>
+      <c r="A422" s="29"/>
     </row>
     <row r="423">
-      <c r="A423" s="22"/>
+      <c r="A423" s="29"/>
     </row>
     <row r="424">
-      <c r="A424" s="22"/>
+      <c r="A424" s="29"/>
     </row>
     <row r="425">
-      <c r="A425" s="22"/>
+      <c r="A425" s="29"/>
     </row>
     <row r="426">
-      <c r="A426" s="22"/>
+      <c r="A426" s="29"/>
     </row>
     <row r="427">
-      <c r="A427" s="22"/>
+      <c r="A427" s="29"/>
     </row>
     <row r="428">
-      <c r="A428" s="22"/>
+      <c r="A428" s="29"/>
     </row>
     <row r="429">
-      <c r="A429" s="22"/>
+      <c r="A429" s="29"/>
     </row>
     <row r="430">
-      <c r="A430" s="22"/>
+      <c r="A430" s="29"/>
     </row>
     <row r="431">
-      <c r="A431" s="22"/>
+      <c r="A431" s="29"/>
     </row>
     <row r="432">
-      <c r="A432" s="22"/>
+      <c r="A432" s="29"/>
     </row>
     <row r="433">
-      <c r="A433" s="22"/>
+      <c r="A433" s="29"/>
     </row>
     <row r="434">
-      <c r="A434" s="22"/>
+      <c r="A434" s="29"/>
     </row>
     <row r="435">
-      <c r="A435" s="22"/>
+      <c r="A435" s="29"/>
     </row>
     <row r="436">
-      <c r="A436" s="22"/>
+      <c r="A436" s="29"/>
     </row>
     <row r="437">
-      <c r="A437" s="22"/>
+      <c r="A437" s="29"/>
     </row>
     <row r="438">
-      <c r="A438" s="22"/>
+      <c r="A438" s="29"/>
     </row>
     <row r="439">
-      <c r="A439" s="22"/>
+      <c r="A439" s="29"/>
     </row>
     <row r="440">
-      <c r="A440" s="22"/>
+      <c r="A440" s="29"/>
     </row>
     <row r="441">
-      <c r="A441" s="22"/>
+      <c r="A441" s="29"/>
     </row>
     <row r="442">
-      <c r="A442" s="22"/>
+      <c r="A442" s="29"/>
     </row>
     <row r="443">
-      <c r="A443" s="22"/>
+      <c r="A443" s="29"/>
     </row>
     <row r="444">
-      <c r="A444" s="22"/>
+      <c r="A444" s="29"/>
     </row>
     <row r="445">
-      <c r="A445" s="22"/>
+      <c r="A445" s="29"/>
     </row>
     <row r="446">
-      <c r="A446" s="22"/>
+      <c r="A446" s="29"/>
     </row>
     <row r="447">
-      <c r="A447" s="22"/>
+      <c r="A447" s="29"/>
     </row>
     <row r="448">
-      <c r="A448" s="22"/>
+      <c r="A448" s="29"/>
     </row>
     <row r="449">
-      <c r="A449" s="22"/>
+      <c r="A449" s="29"/>
     </row>
     <row r="450">
-      <c r="A450" s="22"/>
+      <c r="A450" s="29"/>
     </row>
     <row r="451">
-      <c r="A451" s="22"/>
+      <c r="A451" s="29"/>
     </row>
     <row r="452">
-      <c r="A452" s="22"/>
+      <c r="A452" s="29"/>
     </row>
     <row r="453">
-      <c r="A453" s="22"/>
+      <c r="A453" s="29"/>
     </row>
     <row r="454">
-      <c r="A454" s="22"/>
+      <c r="A454" s="29"/>
     </row>
     <row r="455">
-      <c r="A455" s="22"/>
+      <c r="A455" s="29"/>
     </row>
     <row r="456">
-      <c r="A456" s="22"/>
+      <c r="A456" s="29"/>
     </row>
     <row r="457">
-      <c r="A457" s="22"/>
+      <c r="A457" s="29"/>
     </row>
     <row r="458">
-      <c r="A458" s="22"/>
+      <c r="A458" s="29"/>
     </row>
     <row r="459">
-      <c r="A459" s="22"/>
+      <c r="A459" s="29"/>
     </row>
     <row r="460">
-      <c r="A460" s="22"/>
+      <c r="A460" s="29"/>
     </row>
     <row r="461">
-      <c r="A461" s="22"/>
+      <c r="A461" s="29"/>
     </row>
     <row r="462">
-      <c r="A462" s="22"/>
+      <c r="A462" s="29"/>
     </row>
     <row r="463">
-      <c r="A463" s="22"/>
+      <c r="A463" s="29"/>
     </row>
     <row r="464">
-      <c r="A464" s="22"/>
+      <c r="A464" s="29"/>
     </row>
     <row r="465">
-      <c r="A465" s="22"/>
+      <c r="A465" s="29"/>
     </row>
     <row r="466">
-      <c r="A466" s="22"/>
+      <c r="A466" s="29"/>
     </row>
     <row r="467">
-      <c r="A467" s="22"/>
+      <c r="A467" s="29"/>
     </row>
     <row r="468">
-      <c r="A468" s="22"/>
+      <c r="A468" s="29"/>
     </row>
     <row r="469">
-      <c r="A469" s="22"/>
+      <c r="A469" s="29"/>
     </row>
     <row r="470">
-      <c r="A470" s="22"/>
+      <c r="A470" s="29"/>
     </row>
     <row r="471">
-      <c r="A471" s="22"/>
+      <c r="A471" s="29"/>
     </row>
     <row r="472">
-      <c r="A472" s="22"/>
+      <c r="A472" s="29"/>
     </row>
     <row r="473">
-      <c r="A473" s="22"/>
+      <c r="A473" s="29"/>
     </row>
     <row r="474">
-      <c r="A474" s="22"/>
+      <c r="A474" s="29"/>
     </row>
     <row r="475">
-      <c r="A475" s="22"/>
+      <c r="A475" s="29"/>
     </row>
     <row r="476">
-      <c r="A476" s="22"/>
+      <c r="A476" s="29"/>
     </row>
     <row r="477">
-      <c r="A477" s="22"/>
+      <c r="A477" s="29"/>
     </row>
     <row r="478">
-      <c r="A478" s="22"/>
+      <c r="A478" s="29"/>
     </row>
     <row r="479">
-      <c r="A479" s="22"/>
+      <c r="A479" s="29"/>
     </row>
     <row r="480">
-      <c r="A480" s="22"/>
+      <c r="A480" s="29"/>
     </row>
     <row r="481">
-      <c r="A481" s="22"/>
+      <c r="A481" s="29"/>
     </row>
     <row r="482">
-      <c r="A482" s="22"/>
+      <c r="A482" s="29"/>
     </row>
     <row r="483">
-      <c r="A483" s="22"/>
+      <c r="A483" s="29"/>
     </row>
     <row r="484">
-      <c r="A484" s="22"/>
+      <c r="A484" s="29"/>
     </row>
     <row r="485">
-      <c r="A485" s="22"/>
+      <c r="A485" s="29"/>
     </row>
     <row r="486">
-      <c r="A486" s="22"/>
+      <c r="A486" s="29"/>
     </row>
     <row r="487">
-      <c r="A487" s="22"/>
+      <c r="A487" s="29"/>
     </row>
     <row r="488">
-      <c r="A488" s="22"/>
+      <c r="A488" s="29"/>
     </row>
     <row r="489">
-      <c r="A489" s="22"/>
+      <c r="A489" s="29"/>
     </row>
     <row r="490">
-      <c r="A490" s="22"/>
+      <c r="A490" s="29"/>
     </row>
     <row r="491">
-      <c r="A491" s="22"/>
+      <c r="A491" s="29"/>
     </row>
     <row r="492">
-      <c r="A492" s="22"/>
+      <c r="A492" s="29"/>
     </row>
     <row r="493">
-      <c r="A493" s="22"/>
+      <c r="A493" s="29"/>
     </row>
     <row r="494">
-      <c r="A494" s="22"/>
+      <c r="A494" s="29"/>
     </row>
     <row r="495">
-      <c r="A495" s="22"/>
+      <c r="A495" s="29"/>
     </row>
     <row r="496">
-      <c r="A496" s="22"/>
+      <c r="A496" s="29"/>
     </row>
     <row r="497">
-      <c r="A497" s="22"/>
+      <c r="A497" s="29"/>
     </row>
     <row r="498">
-      <c r="A498" s="22"/>
+      <c r="A498" s="29"/>
     </row>
     <row r="499">
-      <c r="A499" s="22"/>
+      <c r="A499" s="29"/>
     </row>
     <row r="500">
-      <c r="A500" s="22"/>
+      <c r="A500" s="29"/>
     </row>
     <row r="501">
-      <c r="A501" s="22"/>
+      <c r="A501" s="29"/>
     </row>
     <row r="502">
-      <c r="A502" s="22"/>
+      <c r="A502" s="29"/>
     </row>
     <row r="503">
-      <c r="A503" s="22"/>
+      <c r="A503" s="29"/>
     </row>
     <row r="504">
-      <c r="A504" s="22"/>
+      <c r="A504" s="29"/>
     </row>
     <row r="505">
-      <c r="A505" s="22"/>
+      <c r="A505" s="29"/>
     </row>
     <row r="506">
-      <c r="A506" s="22"/>
+      <c r="A506" s="29"/>
     </row>
     <row r="507">
-      <c r="A507" s="22"/>
+      <c r="A507" s="29"/>
     </row>
     <row r="508">
-      <c r="A508" s="22"/>
+      <c r="A508" s="29"/>
     </row>
     <row r="509">
-      <c r="A509" s="22"/>
+      <c r="A509" s="29"/>
     </row>
     <row r="510">
-      <c r="A510" s="22"/>
+      <c r="A510" s="29"/>
     </row>
     <row r="511">
-      <c r="A511" s="22"/>
+      <c r="A511" s="29"/>
     </row>
     <row r="512">
-      <c r="A512" s="22"/>
+      <c r="A512" s="29"/>
     </row>
     <row r="513">
-      <c r="A513" s="22"/>
+      <c r="A513" s="29"/>
     </row>
     <row r="514">
-      <c r="A514" s="22"/>
+      <c r="A514" s="29"/>
     </row>
     <row r="515">
-      <c r="A515" s="22"/>
+      <c r="A515" s="29"/>
     </row>
     <row r="516">
-      <c r="A516" s="22"/>
+      <c r="A516" s="29"/>
     </row>
     <row r="517">
-      <c r="A517" s="22"/>
+      <c r="A517" s="29"/>
     </row>
     <row r="518">
-      <c r="A518" s="22"/>
+      <c r="A518" s="29"/>
     </row>
     <row r="519">
-      <c r="A519" s="22"/>
+      <c r="A519" s="29"/>
     </row>
     <row r="520">
-      <c r="A520" s="22"/>
+      <c r="A520" s="29"/>
     </row>
     <row r="521">
-      <c r="A521" s="22"/>
+      <c r="A521" s="29"/>
     </row>
     <row r="522">
-      <c r="A522" s="22"/>
+      <c r="A522" s="29"/>
     </row>
     <row r="523">
-      <c r="A523" s="22"/>
+      <c r="A523" s="29"/>
     </row>
     <row r="524">
-      <c r="A524" s="22"/>
+      <c r="A524" s="29"/>
     </row>
     <row r="525">
-      <c r="A525" s="22"/>
+      <c r="A525" s="29"/>
     </row>
     <row r="526">
-      <c r="A526" s="22"/>
+      <c r="A526" s="29"/>
     </row>
     <row r="527">
-      <c r="A527" s="22"/>
+      <c r="A527" s="29"/>
     </row>
     <row r="528">
-      <c r="A528" s="22"/>
+      <c r="A528" s="29"/>
     </row>
     <row r="529">
-      <c r="A529" s="22"/>
+      <c r="A529" s="29"/>
     </row>
     <row r="530">
-      <c r="A530" s="22"/>
+      <c r="A530" s="29"/>
     </row>
     <row r="531">
-      <c r="A531" s="22"/>
+      <c r="A531" s="29"/>
     </row>
     <row r="532">
-      <c r="A532" s="22"/>
+      <c r="A532" s="29"/>
     </row>
     <row r="533">
-      <c r="A533" s="22"/>
+      <c r="A533" s="29"/>
     </row>
     <row r="534">
-      <c r="A534" s="22"/>
+      <c r="A534" s="29"/>
     </row>
     <row r="535">
-      <c r="A535" s="22"/>
+      <c r="A535" s="29"/>
     </row>
     <row r="536">
-      <c r="A536" s="22"/>
+      <c r="A536" s="29"/>
     </row>
     <row r="537">
-      <c r="A537" s="22"/>
+      <c r="A537" s="29"/>
     </row>
     <row r="538">
-      <c r="A538" s="22"/>
+      <c r="A538" s="29"/>
     </row>
     <row r="539">
-      <c r="A539" s="22"/>
+      <c r="A539" s="29"/>
     </row>
     <row r="540">
-      <c r="A540" s="22"/>
+      <c r="A540" s="29"/>
     </row>
     <row r="541">
-      <c r="A541" s="22"/>
+      <c r="A541" s="29"/>
     </row>
     <row r="542">
-      <c r="A542" s="22"/>
+      <c r="A542" s="29"/>
     </row>
     <row r="543">
-      <c r="A543" s="22"/>
+      <c r="A543" s="29"/>
     </row>
     <row r="544">
-      <c r="A544" s="22"/>
+      <c r="A544" s="29"/>
     </row>
     <row r="545">
-      <c r="A545" s="22"/>
+      <c r="A545" s="29"/>
     </row>
     <row r="546">
-      <c r="A546" s="22"/>
+      <c r="A546" s="29"/>
     </row>
     <row r="547">
-      <c r="A547" s="22"/>
+      <c r="A547" s="29"/>
     </row>
     <row r="548">
-      <c r="A548" s="22"/>
+      <c r="A548" s="29"/>
     </row>
     <row r="549">
-      <c r="A549" s="22"/>
+      <c r="A549" s="29"/>
     </row>
     <row r="550">
-      <c r="A550" s="22"/>
+      <c r="A550" s="29"/>
     </row>
     <row r="551">
-      <c r="A551" s="22"/>
+      <c r="A551" s="29"/>
     </row>
     <row r="552">
-      <c r="A552" s="22"/>
+      <c r="A552" s="29"/>
     </row>
     <row r="553">
-      <c r="A553" s="22"/>
+      <c r="A553" s="29"/>
     </row>
     <row r="554">
-      <c r="A554" s="22"/>
+      <c r="A554" s="29"/>
     </row>
     <row r="555">
-      <c r="A555" s="22"/>
+      <c r="A555" s="29"/>
     </row>
     <row r="556">
-      <c r="A556" s="22"/>
+      <c r="A556" s="29"/>
     </row>
     <row r="557">
-      <c r="A557" s="22"/>
+      <c r="A557" s="29"/>
     </row>
     <row r="558">
-      <c r="A558" s="22"/>
+      <c r="A558" s="29"/>
     </row>
     <row r="559">
-      <c r="A559" s="22"/>
+      <c r="A559" s="29"/>
     </row>
     <row r="560">
-      <c r="A560" s="22"/>
+      <c r="A560" s="29"/>
     </row>
     <row r="561">
-      <c r="A561" s="22"/>
+      <c r="A561" s="29"/>
     </row>
     <row r="562">
-      <c r="A562" s="22"/>
+      <c r="A562" s="29"/>
     </row>
     <row r="563">
-      <c r="A563" s="22"/>
+      <c r="A563" s="29"/>
     </row>
     <row r="564">
-      <c r="A564" s="22"/>
+      <c r="A564" s="29"/>
     </row>
     <row r="565">
-      <c r="A565" s="22"/>
+      <c r="A565" s="29"/>
     </row>
     <row r="566">
-      <c r="A566" s="22"/>
+      <c r="A566" s="29"/>
     </row>
     <row r="567">
-      <c r="A567" s="22"/>
+      <c r="A567" s="29"/>
     </row>
     <row r="568">
-      <c r="A568" s="22"/>
+      <c r="A568" s="29"/>
     </row>
     <row r="569">
-      <c r="A569" s="22"/>
+      <c r="A569" s="29"/>
     </row>
     <row r="570">
-      <c r="A570" s="22"/>
+      <c r="A570" s="29"/>
     </row>
     <row r="571">
-      <c r="A571" s="22"/>
+      <c r="A571" s="29"/>
     </row>
     <row r="572">
-      <c r="A572" s="22"/>
+      <c r="A572" s="29"/>
     </row>
     <row r="573">
-      <c r="A573" s="22"/>
+      <c r="A573" s="29"/>
     </row>
     <row r="574">
-      <c r="A574" s="22"/>
+      <c r="A574" s="29"/>
     </row>
     <row r="575">
-      <c r="A575" s="22"/>
+      <c r="A575" s="29"/>
     </row>
     <row r="576">
-      <c r="A576" s="22"/>
+      <c r="A576" s="29"/>
     </row>
     <row r="577">
-      <c r="A577" s="22"/>
+      <c r="A577" s="29"/>
     </row>
     <row r="578">
-      <c r="A578" s="22"/>
+      <c r="A578" s="29"/>
     </row>
     <row r="579">
-      <c r="A579" s="22"/>
+      <c r="A579" s="29"/>
     </row>
     <row r="580">
-      <c r="A580" s="22"/>
+      <c r="A580" s="29"/>
     </row>
     <row r="581">
-      <c r="A581" s="22"/>
+      <c r="A581" s="29"/>
     </row>
     <row r="582">
-      <c r="A582" s="22"/>
+      <c r="A582" s="29"/>
     </row>
     <row r="583">
-      <c r="A583" s="22"/>
+      <c r="A583" s="29"/>
     </row>
     <row r="584">
-      <c r="A584" s="22"/>
+      <c r="A584" s="29"/>
     </row>
     <row r="585">
-      <c r="A585" s="22"/>
+      <c r="A585" s="29"/>
     </row>
     <row r="586">
-      <c r="A586" s="22"/>
+      <c r="A586" s="29"/>
     </row>
     <row r="587">
-      <c r="A587" s="22"/>
+      <c r="A587" s="29"/>
     </row>
     <row r="588">
-      <c r="A588" s="22"/>
+      <c r="A588" s="29"/>
     </row>
     <row r="589">
-      <c r="A589" s="22"/>
+      <c r="A589" s="29"/>
     </row>
     <row r="590">
-      <c r="A590" s="22"/>
+      <c r="A590" s="29"/>
     </row>
     <row r="591">
-      <c r="A591" s="22"/>
+      <c r="A591" s="29"/>
     </row>
     <row r="592">
-      <c r="A592" s="22"/>
+      <c r="A592" s="29"/>
     </row>
     <row r="593">
-      <c r="A593" s="22"/>
+      <c r="A593" s="29"/>
     </row>
     <row r="594">
-      <c r="A594" s="22"/>
+      <c r="A594" s="29"/>
     </row>
     <row r="595">
-      <c r="A595" s="22"/>
+      <c r="A595" s="29"/>
     </row>
     <row r="596">
-      <c r="A596" s="22"/>
+      <c r="A596" s="29"/>
     </row>
     <row r="597">
-      <c r="A597" s="22"/>
+      <c r="A597" s="29"/>
     </row>
     <row r="598">
-      <c r="A598" s="22"/>
+      <c r="A598" s="29"/>
     </row>
     <row r="599">
-      <c r="A599" s="22"/>
+      <c r="A599" s="29"/>
     </row>
     <row r="600">
-      <c r="A600" s="22"/>
+      <c r="A600" s="29"/>
     </row>
     <row r="601">
-      <c r="A601" s="22"/>
+      <c r="A601" s="29"/>
     </row>
     <row r="602">
-      <c r="A602" s="22"/>
+      <c r="A602" s="29"/>
     </row>
     <row r="603">
-      <c r="A603" s="22"/>
+      <c r="A603" s="29"/>
     </row>
     <row r="604">
-      <c r="A604" s="22"/>
+      <c r="A604" s="29"/>
     </row>
     <row r="605">
-      <c r="A605" s="22"/>
+      <c r="A605" s="29"/>
     </row>
     <row r="606">
-      <c r="A606" s="22"/>
+      <c r="A606" s="29"/>
     </row>
     <row r="607">
-      <c r="A607" s="22"/>
+      <c r="A607" s="29"/>
     </row>
     <row r="608">
-      <c r="A608" s="22"/>
+      <c r="A608" s="29"/>
     </row>
     <row r="609">
-      <c r="A609" s="22"/>
+      <c r="A609" s="29"/>
     </row>
     <row r="610">
-      <c r="A610" s="22"/>
+      <c r="A610" s="29"/>
     </row>
     <row r="611">
-      <c r="A611" s="22"/>
+      <c r="A611" s="29"/>
     </row>
     <row r="612">
-      <c r="A612" s="22"/>
+      <c r="A612" s="29"/>
     </row>
     <row r="613">
-      <c r="A613" s="22"/>
+      <c r="A613" s="29"/>
     </row>
     <row r="614">
-      <c r="A614" s="22"/>
+      <c r="A614" s="29"/>
     </row>
     <row r="615">
-      <c r="A615" s="22"/>
+      <c r="A615" s="29"/>
     </row>
     <row r="616">
-      <c r="A616" s="22"/>
+      <c r="A616" s="29"/>
     </row>
     <row r="617">
-      <c r="A617" s="22"/>
+      <c r="A617" s="29"/>
     </row>
     <row r="618">
-      <c r="A618" s="22"/>
+      <c r="A618" s="29"/>
     </row>
     <row r="619">
-      <c r="A619" s="22"/>
+      <c r="A619" s="29"/>
     </row>
     <row r="620">
-      <c r="A620" s="22"/>
+      <c r="A620" s="29"/>
     </row>
     <row r="621">
-      <c r="A621" s="22"/>
+      <c r="A621" s="29"/>
     </row>
     <row r="622">
-      <c r="A622" s="22"/>
+      <c r="A622" s="29"/>
     </row>
     <row r="623">
-      <c r="A623" s="22"/>
+      <c r="A623" s="29"/>
     </row>
     <row r="624">
-      <c r="A624" s="22"/>
+      <c r="A624" s="29"/>
     </row>
     <row r="625">
-      <c r="A625" s="22"/>
+      <c r="A625" s="29"/>
     </row>
     <row r="626">
-      <c r="A626" s="22"/>
+      <c r="A626" s="29"/>
     </row>
     <row r="627">
-      <c r="A627" s="22"/>
+      <c r="A627" s="29"/>
     </row>
     <row r="628">
-      <c r="A628" s="22"/>
+      <c r="A628" s="29"/>
     </row>
     <row r="629">
-      <c r="A629" s="22"/>
+      <c r="A629" s="29"/>
     </row>
     <row r="630">
-      <c r="A630" s="22"/>
+      <c r="A630" s="29"/>
     </row>
     <row r="631">
-      <c r="A631" s="22"/>
+      <c r="A631" s="29"/>
     </row>
     <row r="632">
-      <c r="A632" s="22"/>
+      <c r="A632" s="29"/>
     </row>
     <row r="633">
-      <c r="A633" s="22"/>
+      <c r="A633" s="29"/>
     </row>
     <row r="634">
-      <c r="A634" s="22"/>
+      <c r="A634" s="29"/>
     </row>
     <row r="635">
-      <c r="A635" s="22"/>
+      <c r="A635" s="29"/>
     </row>
     <row r="636">
-      <c r="A636" s="22"/>
+      <c r="A636" s="29"/>
     </row>
     <row r="637">
-      <c r="A637" s="22"/>
+      <c r="A637" s="29"/>
     </row>
     <row r="638">
-      <c r="A638" s="22"/>
+      <c r="A638" s="29"/>
     </row>
     <row r="639">
-      <c r="A639" s="22"/>
+      <c r="A639" s="29"/>
     </row>
     <row r="640">
-      <c r="A640" s="22"/>
+      <c r="A640" s="29"/>
     </row>
     <row r="641">
-      <c r="A641" s="22"/>
+      <c r="A641" s="29"/>
     </row>
     <row r="642">
-      <c r="A642" s="22"/>
+      <c r="A642" s="29"/>
     </row>
     <row r="643">
-      <c r="A643" s="22"/>
+      <c r="A643" s="29"/>
     </row>
     <row r="644">
-      <c r="A644" s="22"/>
+      <c r="A644" s="29"/>
     </row>
     <row r="645">
-      <c r="A645" s="22"/>
+      <c r="A645" s="29"/>
     </row>
     <row r="646">
-      <c r="A646" s="22"/>
+      <c r="A646" s="29"/>
     </row>
     <row r="647">
-      <c r="A647" s="22"/>
+      <c r="A647" s="29"/>
     </row>
     <row r="648">
-      <c r="A648" s="22"/>
+      <c r="A648" s="29"/>
     </row>
     <row r="649">
-      <c r="A649" s="22"/>
+      <c r="A649" s="29"/>
     </row>
     <row r="650">
-      <c r="A650" s="22"/>
+      <c r="A650" s="29"/>
     </row>
     <row r="651">
-      <c r="A651" s="22"/>
+      <c r="A651" s="29"/>
     </row>
     <row r="652">
-      <c r="A652" s="22"/>
+      <c r="A652" s="29"/>
     </row>
     <row r="653">
-      <c r="A653" s="22"/>
+      <c r="A653" s="29"/>
     </row>
     <row r="654">
-      <c r="A654" s="22"/>
+      <c r="A654" s="29"/>
     </row>
     <row r="655">
-      <c r="A655" s="22"/>
+      <c r="A655" s="29"/>
     </row>
     <row r="656">
-      <c r="A656" s="22"/>
+      <c r="A656" s="29"/>
     </row>
     <row r="657">
-      <c r="A657" s="22"/>
+      <c r="A657" s="29"/>
     </row>
     <row r="658">
-      <c r="A658" s="22"/>
+      <c r="A658" s="29"/>
     </row>
     <row r="659">
-      <c r="A659" s="22"/>
+      <c r="A659" s="29"/>
     </row>
     <row r="660">
-      <c r="A660" s="22"/>
+      <c r="A660" s="29"/>
     </row>
     <row r="661">
-      <c r="A661" s="22"/>
+      <c r="A661" s="29"/>
     </row>
     <row r="662">
-      <c r="A662" s="22"/>
+      <c r="A662" s="29"/>
     </row>
     <row r="663">
-      <c r="A663" s="22"/>
+      <c r="A663" s="29"/>
     </row>
     <row r="664">
-      <c r="A664" s="22"/>
+      <c r="A664" s="29"/>
     </row>
     <row r="665">
-      <c r="A665" s="22"/>
+      <c r="A665" s="29"/>
     </row>
     <row r="666">
-      <c r="A666" s="22"/>
+      <c r="A666" s="29"/>
     </row>
     <row r="667">
-      <c r="A667" s="22"/>
+      <c r="A667" s="29"/>
     </row>
     <row r="668">
-      <c r="A668" s="22"/>
+      <c r="A668" s="29"/>
     </row>
     <row r="669">
-      <c r="A669" s="22"/>
+      <c r="A669" s="29"/>
     </row>
     <row r="670">
-      <c r="A670" s="22"/>
+      <c r="A670" s="29"/>
     </row>
     <row r="671">
-      <c r="A671" s="22"/>
+      <c r="A671" s="29"/>
     </row>
     <row r="672">
-      <c r="A672" s="22"/>
+      <c r="A672" s="29"/>
     </row>
     <row r="673">
-      <c r="A673" s="22"/>
+      <c r="A673" s="29"/>
     </row>
     <row r="674">
-      <c r="A674" s="22"/>
+      <c r="A674" s="29"/>
     </row>
     <row r="675">
-      <c r="A675" s="22"/>
+      <c r="A675" s="29"/>
     </row>
     <row r="676">
-      <c r="A676" s="22"/>
+      <c r="A676" s="29"/>
     </row>
     <row r="677">
-      <c r="A677" s="22"/>
+      <c r="A677" s="29"/>
     </row>
     <row r="678">
-      <c r="A678" s="22"/>
+      <c r="A678" s="29"/>
     </row>
     <row r="679">
-      <c r="A679" s="22"/>
+      <c r="A679" s="29"/>
     </row>
     <row r="680">
-      <c r="A680" s="22"/>
+      <c r="A680" s="29"/>
     </row>
     <row r="681">
-      <c r="A681" s="22"/>
+      <c r="A681" s="29"/>
     </row>
     <row r="682">
-      <c r="A682" s="22"/>
+      <c r="A682" s="29"/>
     </row>
     <row r="683">
-      <c r="A683" s="22"/>
+      <c r="A683" s="29"/>
     </row>
     <row r="684">
-      <c r="A684" s="22"/>
+      <c r="A684" s="29"/>
     </row>
     <row r="685">
-      <c r="A685" s="22"/>
+      <c r="A685" s="29"/>
     </row>
     <row r="686">
-      <c r="A686" s="22"/>
+      <c r="A686" s="29"/>
     </row>
     <row r="687">
-      <c r="A687" s="22"/>
+      <c r="A687" s="29"/>
     </row>
     <row r="688">
-      <c r="A688" s="22"/>
+      <c r="A688" s="29"/>
     </row>
     <row r="689">
-      <c r="A689" s="22"/>
+      <c r="A689" s="29"/>
     </row>
     <row r="690">
-      <c r="A690" s="22"/>
+      <c r="A690" s="29"/>
     </row>
     <row r="691">
-      <c r="A691" s="22"/>
+      <c r="A691" s="29"/>
     </row>
     <row r="692">
-      <c r="A692" s="22"/>
+      <c r="A692" s="29"/>
     </row>
     <row r="693">
-      <c r="A693" s="22"/>
+      <c r="A693" s="29"/>
     </row>
     <row r="694">
-      <c r="A694" s="22"/>
+      <c r="A694" s="29"/>
     </row>
     <row r="695">
-      <c r="A695" s="22"/>
+      <c r="A695" s="29"/>
     </row>
     <row r="696">
-      <c r="A696" s="22"/>
+      <c r="A696" s="29"/>
     </row>
     <row r="697">
-      <c r="A697" s="22"/>
+      <c r="A697" s="29"/>
     </row>
     <row r="698">
-      <c r="A698" s="22"/>
+      <c r="A698" s="29"/>
     </row>
     <row r="699">
-      <c r="A699" s="22"/>
+      <c r="A699" s="29"/>
     </row>
     <row r="700">
-      <c r="A700" s="22"/>
+      <c r="A700" s="29"/>
     </row>
     <row r="701">
-      <c r="A701" s="22"/>
+      <c r="A701" s="29"/>
     </row>
     <row r="702">
-      <c r="A702" s="22"/>
+      <c r="A702" s="29"/>
     </row>
     <row r="703">
-      <c r="A703" s="22"/>
+      <c r="A703" s="29"/>
     </row>
     <row r="704">
-      <c r="A704" s="22"/>
+      <c r="A704" s="29"/>
     </row>
     <row r="705">
-      <c r="A705" s="22"/>
+      <c r="A705" s="29"/>
     </row>
     <row r="706">
-      <c r="A706" s="22"/>
+      <c r="A706" s="29"/>
     </row>
     <row r="707">
-      <c r="A707" s="22"/>
+      <c r="A707" s="29"/>
     </row>
     <row r="708">
-      <c r="A708" s="22"/>
+      <c r="A708" s="29"/>
     </row>
     <row r="709">
-      <c r="A709" s="22"/>
+      <c r="A709" s="29"/>
     </row>
     <row r="710">
-      <c r="A710" s="22"/>
+      <c r="A710" s="29"/>
     </row>
     <row r="711">
-      <c r="A711" s="22"/>
+      <c r="A711" s="29"/>
     </row>
     <row r="712">
-      <c r="A712" s="22"/>
+      <c r="A712" s="29"/>
     </row>
     <row r="713">
-      <c r="A713" s="22"/>
+      <c r="A713" s="29"/>
     </row>
     <row r="714">
-      <c r="A714" s="22"/>
+      <c r="A714" s="29"/>
     </row>
     <row r="715">
-      <c r="A715" s="22"/>
+      <c r="A715" s="29"/>
     </row>
     <row r="716">
-      <c r="A716" s="22"/>
+      <c r="A716" s="29"/>
     </row>
     <row r="717">
-      <c r="A717" s="22"/>
+      <c r="A717" s="29"/>
     </row>
     <row r="718">
-      <c r="A718" s="22"/>
+      <c r="A718" s="29"/>
     </row>
     <row r="719">
-      <c r="A719" s="22"/>
+      <c r="A719" s="29"/>
     </row>
     <row r="720">
-      <c r="A720" s="22"/>
+      <c r="A720" s="29"/>
     </row>
     <row r="721">
-      <c r="A721" s="22"/>
+      <c r="A721" s="29"/>
     </row>
     <row r="722">
-      <c r="A722" s="22"/>
+      <c r="A722" s="29"/>
     </row>
     <row r="723">
-      <c r="A723" s="22"/>
+      <c r="A723" s="29"/>
     </row>
     <row r="724">
-      <c r="A724" s="22"/>
+      <c r="A724" s="29"/>
     </row>
     <row r="725">
-      <c r="A725" s="22"/>
+      <c r="A725" s="29"/>
     </row>
     <row r="726">
-      <c r="A726" s="22"/>
+      <c r="A726" s="29"/>
     </row>
     <row r="727">
-      <c r="A727" s="22"/>
+      <c r="A727" s="29"/>
     </row>
     <row r="728">
-      <c r="A728" s="22"/>
+      <c r="A728" s="29"/>
     </row>
     <row r="729">
-      <c r="A729" s="22"/>
+      <c r="A729" s="29"/>
     </row>
     <row r="730">
-      <c r="A730" s="22"/>
+      <c r="A730" s="29"/>
     </row>
     <row r="731">
-      <c r="A731" s="22"/>
+      <c r="A731" s="29"/>
     </row>
     <row r="732">
-      <c r="A732" s="22"/>
+      <c r="A732" s="29"/>
     </row>
     <row r="733">
-      <c r="A733" s="22"/>
+      <c r="A733" s="29"/>
     </row>
     <row r="734">
-      <c r="A734" s="22"/>
+      <c r="A734" s="29"/>
     </row>
     <row r="735">
-      <c r="A735" s="22"/>
+      <c r="A735" s="29"/>
     </row>
     <row r="736">
-      <c r="A736" s="22"/>
+      <c r="A736" s="29"/>
     </row>
     <row r="737">
-      <c r="A737" s="22"/>
+      <c r="A737" s="29"/>
     </row>
     <row r="738">
-      <c r="A738" s="22"/>
+      <c r="A738" s="29"/>
     </row>
     <row r="739">
-      <c r="A739" s="22"/>
+      <c r="A739" s="29"/>
     </row>
     <row r="740">
-      <c r="A740" s="22"/>
+      <c r="A740" s="29"/>
     </row>
     <row r="741">
-      <c r="A741" s="22"/>
+      <c r="A741" s="29"/>
     </row>
     <row r="742">
-      <c r="A742" s="22"/>
+      <c r="A742" s="29"/>
     </row>
     <row r="743">
-      <c r="A743" s="22"/>
+      <c r="A743" s="29"/>
     </row>
     <row r="744">
-      <c r="A744" s="22"/>
+      <c r="A744" s="29"/>
     </row>
     <row r="745">
-      <c r="A745" s="22"/>
+      <c r="A745" s="29"/>
     </row>
     <row r="746">
-      <c r="A746" s="22"/>
+      <c r="A746" s="29"/>
     </row>
     <row r="747">
-      <c r="A747" s="22"/>
+      <c r="A747" s="29"/>
     </row>
     <row r="748">
-      <c r="A748" s="22"/>
+      <c r="A748" s="29"/>
     </row>
     <row r="749">
-      <c r="A749" s="22"/>
+      <c r="A749" s="29"/>
     </row>
     <row r="750">
-      <c r="A750" s="22"/>
+      <c r="A750" s="29"/>
     </row>
     <row r="751">
-      <c r="A751" s="22"/>
+      <c r="A751" s="29"/>
     </row>
     <row r="752">
-      <c r="A752" s="22"/>
+      <c r="A752" s="29"/>
     </row>
     <row r="753">
-      <c r="A753" s="22"/>
+      <c r="A753" s="29"/>
     </row>
     <row r="754">
-      <c r="A754" s="22"/>
+      <c r="A754" s="29"/>
     </row>
     <row r="755">
-      <c r="A755" s="22"/>
+      <c r="A755" s="29"/>
     </row>
     <row r="756">
-      <c r="A756" s="22"/>
+      <c r="A756" s="29"/>
     </row>
     <row r="757">
-      <c r="A757" s="22"/>
+      <c r="A757" s="29"/>
     </row>
     <row r="758">
-      <c r="A758" s="22"/>
+      <c r="A758" s="29"/>
     </row>
     <row r="759">
-      <c r="A759" s="22"/>
+      <c r="A759" s="29"/>
     </row>
     <row r="760">
-      <c r="A760" s="22"/>
+      <c r="A760" s="29"/>
     </row>
     <row r="761">
-      <c r="A761" s="22"/>
+      <c r="A761" s="29"/>
     </row>
     <row r="762">
-      <c r="A762" s="22"/>
+      <c r="A762" s="29"/>
     </row>
     <row r="763">
-      <c r="A763" s="22"/>
+      <c r="A763" s="29"/>
     </row>
     <row r="764">
-      <c r="A764" s="22"/>
+      <c r="A764" s="29"/>
     </row>
     <row r="765">
-      <c r="A765" s="22"/>
+      <c r="A765" s="29"/>
     </row>
     <row r="766">
-      <c r="A766" s="22"/>
+      <c r="A766" s="29"/>
     </row>
     <row r="767">
-      <c r="A767" s="22"/>
+      <c r="A767" s="29"/>
     </row>
     <row r="768">
-      <c r="A768" s="22"/>
+      <c r="A768" s="29"/>
     </row>
     <row r="769">
-      <c r="A769" s="22"/>
+      <c r="A769" s="29"/>
     </row>
     <row r="770">
-      <c r="A770" s="22"/>
+      <c r="A770" s="29"/>
     </row>
     <row r="771">
-      <c r="A771" s="22"/>
+      <c r="A771" s="29"/>
     </row>
     <row r="772">
-      <c r="A772" s="22"/>
+      <c r="A772" s="29"/>
     </row>
     <row r="773">
-      <c r="A773" s="22"/>
+      <c r="A773" s="29"/>
     </row>
     <row r="774">
-      <c r="A774" s="22"/>
+      <c r="A774" s="29"/>
     </row>
     <row r="775">
-      <c r="A775" s="22"/>
+      <c r="A775" s="29"/>
     </row>
     <row r="776">
-      <c r="A776" s="22"/>
+      <c r="A776" s="29"/>
     </row>
     <row r="777">
-      <c r="A777" s="22"/>
+      <c r="A777" s="29"/>
     </row>
     <row r="778">
-      <c r="A778" s="22"/>
+      <c r="A778" s="29"/>
     </row>
     <row r="779">
-      <c r="A779" s="22"/>
+      <c r="A779" s="29"/>
     </row>
     <row r="780">
-      <c r="A780" s="22"/>
+      <c r="A780" s="29"/>
     </row>
     <row r="781">
-      <c r="A781" s="22"/>
+      <c r="A781" s="29"/>
     </row>
     <row r="782">
-      <c r="A782" s="22"/>
+      <c r="A782" s="29"/>
     </row>
     <row r="783">
-      <c r="A783" s="22"/>
+      <c r="A783" s="29"/>
     </row>
     <row r="784">
-      <c r="A784" s="22"/>
+      <c r="A784" s="29"/>
     </row>
     <row r="785">
-      <c r="A785" s="22"/>
+      <c r="A785" s="29"/>
     </row>
     <row r="786">
-      <c r="A786" s="22"/>
+      <c r="A786" s="29"/>
     </row>
     <row r="787">
-      <c r="A787" s="22"/>
+      <c r="A787" s="29"/>
     </row>
     <row r="788">
-      <c r="A788" s="22"/>
+      <c r="A788" s="29"/>
     </row>
     <row r="789">
-      <c r="A789" s="22"/>
+      <c r="A789" s="29"/>
     </row>
     <row r="790">
-      <c r="A790" s="22"/>
+      <c r="A790" s="29"/>
     </row>
     <row r="791">
-      <c r="A791" s="22"/>
+      <c r="A791" s="29"/>
     </row>
     <row r="792">
-      <c r="A792" s="22"/>
+      <c r="A792" s="29"/>
     </row>
     <row r="793">
-      <c r="A793" s="22"/>
+      <c r="A793" s="29"/>
     </row>
     <row r="794">
-      <c r="A794" s="22"/>
+      <c r="A794" s="29"/>
     </row>
     <row r="795">
-      <c r="A795" s="22"/>
+      <c r="A795" s="29"/>
     </row>
     <row r="796">
-      <c r="A796" s="22"/>
+      <c r="A796" s="29"/>
     </row>
     <row r="797">
-      <c r="A797" s="22"/>
+      <c r="A797" s="29"/>
     </row>
     <row r="798">
-      <c r="A798" s="22"/>
+      <c r="A798" s="29"/>
     </row>
     <row r="799">
-      <c r="A799" s="22"/>
+      <c r="A799" s="29"/>
     </row>
     <row r="800">
-      <c r="A800" s="22"/>
+      <c r="A800" s="29"/>
     </row>
     <row r="801">
-      <c r="A801" s="22"/>
+      <c r="A801" s="29"/>
     </row>
     <row r="802">
-      <c r="A802" s="22"/>
+      <c r="A802" s="29"/>
     </row>
     <row r="803">
-      <c r="A803" s="22"/>
+      <c r="A803" s="29"/>
     </row>
     <row r="804">
-      <c r="A804" s="22"/>
+      <c r="A804" s="29"/>
     </row>
     <row r="805">
-      <c r="A805" s="22"/>
+      <c r="A805" s="29"/>
     </row>
     <row r="806">
-      <c r="A806" s="22"/>
+      <c r="A806" s="29"/>
     </row>
     <row r="807">
-      <c r="A807" s="22"/>
+      <c r="A807" s="29"/>
     </row>
     <row r="808">
-      <c r="A808" s="22"/>
+      <c r="A808" s="29"/>
     </row>
     <row r="809">
-      <c r="A809" s="22"/>
+      <c r="A809" s="29"/>
     </row>
     <row r="810">
-      <c r="A810" s="22"/>
+      <c r="A810" s="29"/>
     </row>
     <row r="811">
-      <c r="A811" s="22"/>
+      <c r="A811" s="29"/>
     </row>
     <row r="812">
-      <c r="A812" s="22"/>
+      <c r="A812" s="29"/>
     </row>
     <row r="813">
-      <c r="A813" s="22"/>
+      <c r="A813" s="29"/>
     </row>
     <row r="814">
-      <c r="A814" s="22"/>
+      <c r="A814" s="29"/>
     </row>
     <row r="815">
-      <c r="A815" s="22"/>
+      <c r="A815" s="29"/>
     </row>
     <row r="816">
-      <c r="A816" s="22"/>
+      <c r="A816" s="29"/>
     </row>
     <row r="817">
-      <c r="A817" s="22"/>
+      <c r="A817" s="29"/>
     </row>
     <row r="818">
-      <c r="A818" s="22"/>
+      <c r="A818" s="29"/>
     </row>
     <row r="819">
-      <c r="A819" s="22"/>
+      <c r="A819" s="29"/>
     </row>
     <row r="820">
-      <c r="A820" s="22"/>
+      <c r="A820" s="29"/>
     </row>
     <row r="821">
-      <c r="A821" s="22"/>
+      <c r="A821" s="29"/>
     </row>
     <row r="822">
-      <c r="A822" s="22"/>
+      <c r="A822" s="29"/>
     </row>
     <row r="823">
-      <c r="A823" s="22"/>
+      <c r="A823" s="29"/>
     </row>
     <row r="824">
-      <c r="A824" s="22"/>
+      <c r="A824" s="29"/>
     </row>
     <row r="825">
-      <c r="A825" s="22"/>
+      <c r="A825" s="29"/>
     </row>
     <row r="826">
-      <c r="A826" s="22"/>
+      <c r="A826" s="29"/>
     </row>
     <row r="827">
-      <c r="A827" s="22"/>
+      <c r="A827" s="29"/>
     </row>
     <row r="828">
-      <c r="A828" s="22"/>
+      <c r="A828" s="29"/>
     </row>
     <row r="829">
-      <c r="A829" s="22"/>
+      <c r="A829" s="29"/>
     </row>
     <row r="830">
-      <c r="A830" s="22"/>
+      <c r="A830" s="29"/>
     </row>
     <row r="831">
-      <c r="A831" s="22"/>
+      <c r="A831" s="29"/>
     </row>
     <row r="832">
-      <c r="A832" s="22"/>
+      <c r="A832" s="29"/>
     </row>
     <row r="833">
-      <c r="A833" s="22"/>
+      <c r="A833" s="29"/>
     </row>
     <row r="834">
-      <c r="A834" s="22"/>
+      <c r="A834" s="29"/>
     </row>
     <row r="835">
-      <c r="A835" s="22"/>
+      <c r="A835" s="29"/>
     </row>
     <row r="836">
-      <c r="A836" s="22"/>
+      <c r="A836" s="29"/>
     </row>
     <row r="837">
-      <c r="A837" s="22"/>
+      <c r="A837" s="29"/>
     </row>
     <row r="838">
-      <c r="A838" s="22"/>
+      <c r="A838" s="29"/>
     </row>
     <row r="839">
-      <c r="A839" s="22"/>
+      <c r="A839" s="29"/>
     </row>
     <row r="840">
-      <c r="A840" s="22"/>
+      <c r="A840" s="29"/>
     </row>
     <row r="841">
-      <c r="A841" s="22"/>
+      <c r="A841" s="29"/>
     </row>
     <row r="842">
-      <c r="A842" s="22"/>
+      <c r="A842" s="29"/>
     </row>
     <row r="843">
-      <c r="A843" s="22"/>
+      <c r="A843" s="29"/>
     </row>
     <row r="844">
-      <c r="A844" s="22"/>
+      <c r="A844" s="29"/>
     </row>
     <row r="845">
-      <c r="A845" s="22"/>
+      <c r="A845" s="29"/>
     </row>
     <row r="846">
-      <c r="A846" s="22"/>
+      <c r="A846" s="29"/>
     </row>
     <row r="847">
-      <c r="A847" s="22"/>
+      <c r="A847" s="29"/>
     </row>
     <row r="848">
-      <c r="A848" s="22"/>
+      <c r="A848" s="29"/>
     </row>
     <row r="849">
-      <c r="A849" s="22"/>
+      <c r="A849" s="29"/>
     </row>
     <row r="850">
-      <c r="A850" s="22"/>
+      <c r="A850" s="29"/>
     </row>
     <row r="851">
-      <c r="A851" s="22"/>
+      <c r="A851" s="29"/>
     </row>
     <row r="852">
-      <c r="A852" s="22"/>
+      <c r="A852" s="29"/>
     </row>
     <row r="853">
-      <c r="A853" s="22"/>
+      <c r="A853" s="29"/>
     </row>
     <row r="854">
-      <c r="A854" s="22"/>
+      <c r="A854" s="29"/>
     </row>
     <row r="855">
-      <c r="A855" s="22"/>
+      <c r="A855" s="29"/>
     </row>
     <row r="856">
-      <c r="A856" s="22"/>
+      <c r="A856" s="29"/>
     </row>
     <row r="857">
-      <c r="A857" s="22"/>
+      <c r="A857" s="29"/>
     </row>
     <row r="858">
-      <c r="A858" s="22"/>
+      <c r="A858" s="29"/>
     </row>
     <row r="859">
-      <c r="A859" s="22"/>
+      <c r="A859" s="29"/>
     </row>
     <row r="860">
-      <c r="A860" s="22"/>
+      <c r="A860" s="29"/>
     </row>
     <row r="861">
-      <c r="A861" s="22"/>
+      <c r="A861" s="29"/>
     </row>
     <row r="862">
-      <c r="A862" s="22"/>
+      <c r="A862" s="29"/>
     </row>
     <row r="863">
-      <c r="A863" s="22"/>
+      <c r="A863" s="29"/>
     </row>
     <row r="864">
-      <c r="A864" s="22"/>
+      <c r="A864" s="29"/>
     </row>
     <row r="865">
-      <c r="A865" s="22"/>
+      <c r="A865" s="29"/>
     </row>
     <row r="866">
-      <c r="A866" s="22"/>
+      <c r="A866" s="29"/>
     </row>
     <row r="867">
-      <c r="A867" s="22"/>
+      <c r="A867" s="29"/>
     </row>
     <row r="868">
-      <c r="A868" s="22"/>
+      <c r="A868" s="29"/>
     </row>
     <row r="869">
-      <c r="A869" s="22"/>
+      <c r="A869" s="29"/>
     </row>
     <row r="870">
-      <c r="A870" s="22"/>
+      <c r="A870" s="29"/>
     </row>
     <row r="871">
-      <c r="A871" s="22"/>
+      <c r="A871" s="29"/>
     </row>
     <row r="872">
-      <c r="A872" s="22"/>
+      <c r="A872" s="29"/>
     </row>
     <row r="873">
-      <c r="A873" s="22"/>
+      <c r="A873" s="29"/>
     </row>
     <row r="874">
-      <c r="A874" s="22"/>
+      <c r="A874" s="29"/>
     </row>
     <row r="875">
-      <c r="A875" s="22"/>
+      <c r="A875" s="29"/>
     </row>
     <row r="876">
-      <c r="A876" s="22"/>
+      <c r="A876" s="29"/>
     </row>
     <row r="877">
-      <c r="A877" s="22"/>
+      <c r="A877" s="29"/>
     </row>
     <row r="878">
-      <c r="A878" s="22"/>
+      <c r="A878" s="29"/>
     </row>
     <row r="879">
-      <c r="A879" s="22"/>
+      <c r="A879" s="29"/>
     </row>
     <row r="880">
-      <c r="A880" s="22"/>
+      <c r="A880" s="29"/>
     </row>
     <row r="881">
-      <c r="A881" s="22"/>
+      <c r="A881" s="29"/>
     </row>
     <row r="882">
-      <c r="A882" s="22"/>
+      <c r="A882" s="29"/>
     </row>
     <row r="883">
-      <c r="A883" s="22"/>
+      <c r="A883" s="29"/>
     </row>
     <row r="884">
-      <c r="A884" s="22"/>
+      <c r="A884" s="29"/>
     </row>
     <row r="885">
-      <c r="A885" s="22"/>
+      <c r="A885" s="29"/>
     </row>
     <row r="886">
-      <c r="A886" s="22"/>
+      <c r="A886" s="29"/>
     </row>
     <row r="887">
-      <c r="A887" s="22"/>
+      <c r="A887" s="29"/>
     </row>
     <row r="888">
-      <c r="A888" s="22"/>
+      <c r="A888" s="29"/>
     </row>
     <row r="889">
-      <c r="A889" s="22"/>
+      <c r="A889" s="29"/>
     </row>
     <row r="890">
-      <c r="A890" s="22"/>
+      <c r="A890" s="29"/>
     </row>
     <row r="891">
-      <c r="A891" s="22"/>
+      <c r="A891" s="29"/>
     </row>
     <row r="892">
-      <c r="A892" s="22"/>
+      <c r="A892" s="29"/>
     </row>
     <row r="893">
-      <c r="A893" s="22"/>
+      <c r="A893" s="29"/>
     </row>
     <row r="894">
-      <c r="A894" s="22"/>
+      <c r="A894" s="29"/>
     </row>
     <row r="895">
-      <c r="A895" s="22"/>
+      <c r="A895" s="29"/>
     </row>
     <row r="896">
-      <c r="A896" s="22"/>
+      <c r="A896" s="29"/>
     </row>
     <row r="897">
-      <c r="A897" s="22"/>
+      <c r="A897" s="29"/>
     </row>
     <row r="898">
-      <c r="A898" s="22"/>
+      <c r="A898" s="29"/>
     </row>
     <row r="899">
-      <c r="A899" s="22"/>
+      <c r="A899" s="29"/>
     </row>
     <row r="900">
-      <c r="A900" s="22"/>
+      <c r="A900" s="29"/>
     </row>
     <row r="901">
-      <c r="A901" s="22"/>
+      <c r="A901" s="29"/>
     </row>
     <row r="902">
-      <c r="A902" s="22"/>
+      <c r="A902" s="29"/>
     </row>
     <row r="903">
-      <c r="A903" s="22"/>
+      <c r="A903" s="29"/>
     </row>
     <row r="904">
-      <c r="A904" s="22"/>
+      <c r="A904" s="29"/>
     </row>
     <row r="905">
-      <c r="A905" s="22"/>
+      <c r="A905" s="29"/>
     </row>
     <row r="906">
-      <c r="A906" s="22"/>
+      <c r="A906" s="29"/>
     </row>
     <row r="907">
-      <c r="A907" s="22"/>
+      <c r="A907" s="29"/>
     </row>
     <row r="908">
-      <c r="A908" s="22"/>
+      <c r="A908" s="29"/>
     </row>
     <row r="909">
-      <c r="A909" s="22"/>
+      <c r="A909" s="29"/>
     </row>
     <row r="910">
-      <c r="A910" s="22"/>
+      <c r="A910" s="29"/>
     </row>
     <row r="911">
-      <c r="A911" s="22"/>
+      <c r="A911" s="29"/>
     </row>
     <row r="912">
-      <c r="A912" s="22"/>
+      <c r="A912" s="29"/>
     </row>
     <row r="913">
-      <c r="A913" s="22"/>
+      <c r="A913" s="29"/>
     </row>
     <row r="914">
-      <c r="A914" s="22"/>
+      <c r="A914" s="29"/>
     </row>
     <row r="915">
-      <c r="A915" s="22"/>
+      <c r="A915" s="29"/>
     </row>
     <row r="916">
-      <c r="A916" s="22"/>
+      <c r="A916" s="29"/>
     </row>
     <row r="917">
-      <c r="A917" s="22"/>
+      <c r="A917" s="29"/>
     </row>
     <row r="918">
-      <c r="A918" s="22"/>
+      <c r="A918" s="29"/>
     </row>
     <row r="919">
-      <c r="A919" s="22"/>
+      <c r="A919" s="29"/>
     </row>
     <row r="920">
-      <c r="A920" s="22"/>
+      <c r="A920" s="29"/>
     </row>
     <row r="921">
-      <c r="A921" s="22"/>
+      <c r="A921" s="29"/>
     </row>
     <row r="922">
-      <c r="A922" s="22"/>
+      <c r="A922" s="29"/>
     </row>
     <row r="923">
-      <c r="A923" s="22"/>
+      <c r="A923" s="29"/>
     </row>
     <row r="924">
-      <c r="A924" s="22"/>
+      <c r="A924" s="29"/>
     </row>
     <row r="925">
-      <c r="A925" s="22"/>
+      <c r="A925" s="29"/>
     </row>
     <row r="926">
-      <c r="A926" s="22"/>
+      <c r="A926" s="29"/>
     </row>
     <row r="927">
-      <c r="A927" s="22"/>
+      <c r="A927" s="29"/>
     </row>
     <row r="928">
-      <c r="A928" s="22"/>
+      <c r="A928" s="29"/>
     </row>
     <row r="929">
-      <c r="A929" s="22"/>
+      <c r="A929" s="29"/>
     </row>
     <row r="930">
-      <c r="A930" s="22"/>
+      <c r="A930" s="29"/>
     </row>
     <row r="931">
-      <c r="A931" s="22"/>
+      <c r="A931" s="29"/>
     </row>
     <row r="932">
-      <c r="A932" s="22"/>
+      <c r="A932" s="29"/>
     </row>
     <row r="933">
-      <c r="A933" s="22"/>
+      <c r="A933" s="29"/>
     </row>
     <row r="934">
-      <c r="A934" s="22"/>
+      <c r="A934" s="29"/>
     </row>
     <row r="935">
-      <c r="A935" s="22"/>
+      <c r="A935" s="29"/>
     </row>
     <row r="936">
-      <c r="A936" s="22"/>
+      <c r="A936" s="29"/>
     </row>
     <row r="937">
-      <c r="A937" s="22"/>
+      <c r="A937" s="29"/>
     </row>
     <row r="938">
-      <c r="A938" s="22"/>
+      <c r="A938" s="29"/>
     </row>
     <row r="939">
-      <c r="A939" s="22"/>
+      <c r="A939" s="29"/>
     </row>
     <row r="940">
-      <c r="A940" s="22"/>
+      <c r="A940" s="29"/>
     </row>
     <row r="941">
-      <c r="A941" s="22"/>
+      <c r="A941" s="29"/>
     </row>
     <row r="942">
-      <c r="A942" s="22"/>
+      <c r="A942" s="29"/>
     </row>
     <row r="943">
-      <c r="A943" s="22"/>
+      <c r="A943" s="29"/>
     </row>
     <row r="944">
-      <c r="A944" s="22"/>
+      <c r="A944" s="29"/>
     </row>
     <row r="945">
-      <c r="A945" s="22"/>
+      <c r="A945" s="29"/>
     </row>
     <row r="946">
-      <c r="A946" s="22"/>
+      <c r="A946" s="29"/>
     </row>
     <row r="947">
-      <c r="A947" s="22"/>
+      <c r="A947" s="29"/>
     </row>
     <row r="948">
-      <c r="A948" s="22"/>
+      <c r="A948" s="29"/>
     </row>
     <row r="949">
-      <c r="A949" s="22"/>
+      <c r="A949" s="29"/>
     </row>
     <row r="950">
-      <c r="A950" s="22"/>
+      <c r="A950" s="29"/>
     </row>
     <row r="951">
-      <c r="A951" s="22"/>
+      <c r="A951" s="29"/>
     </row>
     <row r="952">
-      <c r="A952" s="22"/>
+      <c r="A952" s="29"/>
     </row>
     <row r="953">
-      <c r="A953" s="22"/>
+      <c r="A953" s="29"/>
     </row>
     <row r="954">
-      <c r="A954" s="22"/>
+      <c r="A954" s="29"/>
     </row>
     <row r="955">
-      <c r="A955" s="22"/>
+      <c r="A955" s="29"/>
     </row>
     <row r="956">
-      <c r="A956" s="22"/>
+      <c r="A956" s="29"/>
     </row>
     <row r="957">
-      <c r="A957" s="22"/>
+      <c r="A957" s="29"/>
     </row>
     <row r="958">
-      <c r="A958" s="22"/>
+      <c r="A958" s="29"/>
     </row>
     <row r="959">
-      <c r="A959" s="22"/>
+      <c r="A959" s="29"/>
     </row>
     <row r="960">
-      <c r="A960" s="22"/>
+      <c r="A960" s="29"/>
     </row>
     <row r="961">
-      <c r="A961" s="22"/>
+      <c r="A961" s="29"/>
     </row>
     <row r="962">
-      <c r="A962" s="22"/>
+      <c r="A962" s="29"/>
     </row>
     <row r="963">
-      <c r="A963" s="22"/>
+      <c r="A963" s="29"/>
     </row>
     <row r="964">
-      <c r="A964" s="22"/>
+      <c r="A964" s="29"/>
     </row>
     <row r="965">
-      <c r="A965" s="22"/>
+      <c r="A965" s="29"/>
     </row>
     <row r="966">
-      <c r="A966" s="22"/>
+      <c r="A966" s="29"/>
     </row>
     <row r="967">
-      <c r="A967" s="22"/>
+      <c r="A967" s="29"/>
     </row>
     <row r="968">
-      <c r="A968" s="22"/>
+      <c r="A968" s="29"/>
     </row>
     <row r="969">
-      <c r="A969" s="22"/>
+      <c r="A969" s="29"/>
     </row>
     <row r="970">
-      <c r="A970" s="22"/>
+      <c r="A970" s="29"/>
     </row>
     <row r="971">
-      <c r="A971" s="22"/>
+      <c r="A971" s="29"/>
     </row>
     <row r="972">
-      <c r="A972" s="22"/>
+      <c r="A972" s="29"/>
     </row>
     <row r="973">
-      <c r="A973" s="22"/>
+      <c r="A973" s="29"/>
     </row>
     <row r="974">
-      <c r="A974" s="22"/>
+      <c r="A974" s="29"/>
     </row>
     <row r="975">
-      <c r="A975" s="22"/>
+      <c r="A975" s="29"/>
     </row>
     <row r="976">
-      <c r="A976" s="22"/>
+      <c r="A976" s="29"/>
     </row>
     <row r="977">
-      <c r="A977" s="22"/>
+      <c r="A977" s="29"/>
     </row>
     <row r="978">
-      <c r="A978" s="22"/>
+      <c r="A978" s="29"/>
     </row>
     <row r="979">
-      <c r="A979" s="22"/>
+      <c r="A979" s="29"/>
     </row>
     <row r="980">
-      <c r="A980" s="22"/>
+      <c r="A980" s="29"/>
     </row>
     <row r="981">
-      <c r="A981" s="22"/>
+      <c r="A981" s="29"/>
     </row>
     <row r="982">
-      <c r="A982" s="22"/>
+      <c r="A982" s="29"/>
     </row>
     <row r="983">
-      <c r="A983" s="22"/>
+      <c r="A983" s="29"/>
     </row>
     <row r="984">
-      <c r="A984" s="22"/>
+      <c r="A984" s="29"/>
     </row>
     <row r="985">
-      <c r="A985" s="22"/>
+      <c r="A985" s="29"/>
     </row>
     <row r="986">
-      <c r="A986" s="22"/>
+      <c r="A986" s="29"/>
     </row>
     <row r="987">
-      <c r="A987" s="22"/>
+      <c r="A987" s="29"/>
     </row>
     <row r="988">
-      <c r="A988" s="22"/>
+      <c r="A988" s="29"/>
     </row>
     <row r="989">
-      <c r="A989" s="22"/>
+      <c r="A989" s="29"/>
     </row>
     <row r="990">
-      <c r="A990" s="22"/>
+      <c r="A990" s="29"/>
     </row>
     <row r="991">
-      <c r="A991" s="22"/>
+      <c r="A991" s="29"/>
     </row>
     <row r="992">
-      <c r="A992" s="22"/>
+      <c r="A992" s="29"/>
     </row>
     <row r="993">
-      <c r="A993" s="22"/>
+      <c r="A993" s="29"/>
     </row>
     <row r="994">
-      <c r="A994" s="22"/>
+      <c r="A994" s="29"/>
     </row>
     <row r="995">
-      <c r="A995" s="22"/>
+      <c r="A995" s="29"/>
     </row>
     <row r="996">
-      <c r="A996" s="22"/>
+      <c r="A996" s="29"/>
     </row>
     <row r="997">
-      <c r="A997" s="22"/>
+      <c r="A997" s="29"/>
     </row>
     <row r="998">
-      <c r="A998" s="22"/>
+      <c r="A998" s="29"/>
     </row>
     <row r="999">
-      <c r="A999" s="22"/>
+      <c r="A999" s="29"/>
     </row>
     <row r="1000">
-      <c r="A1000" s="22"/>
+      <c r="A1000" s="29"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>